<commit_message>
Add Moto3 and Moto2 qualifying and races for GB
</commit_message>
<xml_diff>
--- a/motogp/MotoGP.xlsx
+++ b/motogp/MotoGP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/motogp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0240F0AD-5655-8D4F-BB28-CF8A5232527D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8BF9758-9F3B-8C41-A618-F7F5D903A373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="1900" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="117">
   <si>
     <t>Country</t>
   </si>
@@ -776,11 +776,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A264AA3C-A8BA-6F48-8FC0-C3E78D3BD742}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD32"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1253,7 +1251,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" ref="D14:D42" si="22">VLOOKUP(A14,locations,4)</f>
+        <f t="shared" ref="D14:D46" si="22">VLOOKUP(A14,locations,4)</f>
         <v>Europe/Madrid</v>
       </c>
       <c r="E14" s="4">
@@ -1834,18 +1832,18 @@
         <v>0.4513888888888889</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" ref="G30:G38" si="45">E30</f>
+        <f t="shared" ref="G30:G42" si="45">E30</f>
         <v>45143</v>
       </c>
       <c r="H30" s="6">
         <v>0.47916666666666669</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" ref="I30:I31" si="46">VLOOKUP(A30,locations,2)</f>
+        <f t="shared" ref="I30:I33" si="46">VLOOKUP(A30,locations,2)</f>
         <v>Silverstone</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" ref="J30:J31" si="47">VLOOKUP(A30,locations,3)</f>
+        <f t="shared" ref="J30:J33" si="47">VLOOKUP(A30,locations,3)</f>
         <v>Monster Energy British Grand Prix</v>
       </c>
     </row>
@@ -1854,10 +1852,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="22"/>
@@ -1867,21 +1865,21 @@
         <v>45143</v>
       </c>
       <c r="F31" s="6">
-        <v>0.625</v>
+        <v>0.53472222222222221</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="45"/>
         <v>45143</v>
       </c>
       <c r="H31" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="I31" si="48">VLOOKUP(A31,locations,2)</f>
         <v>Silverstone</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" ref="J31" si="49">VLOOKUP(A31,locations,3)</f>
         <v>Monster Energy British Grand Prix</v>
       </c>
     </row>
@@ -1890,1266 +1888,1410 @@
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D32" t="str">
+        <f t="shared" ref="D32" si="50">VLOOKUP(A32,locations,4)</f>
+        <v>Europe/London</v>
+      </c>
+      <c r="E32" s="4">
+        <v>45143</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" ref="G32" si="51">E32</f>
+        <v>45143</v>
+      </c>
+      <c r="H32" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" ref="I32" si="52">VLOOKUP(A32,locations,2)</f>
+        <v>Silverstone</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" ref="J32" si="53">VLOOKUP(A32,locations,3)</f>
+        <v>Monster Energy British Grand Prix</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" t="str">
         <f t="shared" si="22"/>
         <v>Europe/London</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E33" s="4">
+        <v>45143</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="45"/>
+        <v>45143</v>
+      </c>
+      <c r="H33" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="46"/>
+        <v>Silverstone</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="47"/>
+        <v>Monster Energy British Grand Prix</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" ref="D34" si="54">VLOOKUP(A34,locations,4)</f>
+        <v>Europe/London</v>
+      </c>
+      <c r="E34" s="4">
         <v>45144</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F34" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" ref="G34" si="55">E34</f>
+        <v>45144</v>
+      </c>
+      <c r="H34" s="6">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" ref="I34" si="56">VLOOKUP(A34,locations,2)</f>
+        <v>Silverstone</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" ref="J34" si="57">VLOOKUP(A34,locations,3)</f>
+        <v>Monster Energy British Grand Prix</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="22"/>
+        <v>Europe/London</v>
+      </c>
+      <c r="E35" s="4">
+        <v>45144</v>
+      </c>
+      <c r="F35" s="6">
         <v>0.54166666666666663</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G35" s="4">
         <f t="shared" si="45"/>
         <v>45144</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H35" s="6">
         <v>0.57638888888888895</v>
       </c>
-      <c r="I32" t="str">
-        <f t="shared" ref="I32" si="48">VLOOKUP(A32,locations,2)</f>
+      <c r="I35" t="str">
+        <f t="shared" ref="I35" si="58">VLOOKUP(A35,locations,2)</f>
         <v>Silverstone</v>
       </c>
-      <c r="J32" t="str">
-        <f t="shared" ref="J32" si="49">VLOOKUP(A32,locations,3)</f>
+      <c r="J35" t="str">
+        <f t="shared" ref="J35" si="59">VLOOKUP(A35,locations,3)</f>
         <v>Monster Energy British Grand Prix</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" ref="D36" si="60">VLOOKUP(A36,locations,4)</f>
+        <v>Europe/London</v>
+      </c>
+      <c r="E36" s="4">
+        <v>45144</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G36" s="4">
+        <f t="shared" ref="G36" si="61">E36</f>
+        <v>45144</v>
+      </c>
+      <c r="H36" s="6">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" ref="I36" si="62">VLOOKUP(A36,locations,2)</f>
+        <v>Silverstone</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" ref="J36" si="63">VLOOKUP(A36,locations,3)</f>
+        <v>Monster Energy British Grand Prix</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D33" t="str">
+      <c r="D37" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Vienna</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E37" s="4">
         <v>45157</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F37" s="6">
         <v>0.4513888888888889</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G37" s="4">
         <f t="shared" si="45"/>
         <v>45157</v>
       </c>
-      <c r="H33" s="6">
+      <c r="H37" s="6">
         <v>0.47916666666666669</v>
       </c>
-      <c r="I33" t="str">
-        <f t="shared" ref="I33:I34" si="50">VLOOKUP(A33,locations,2)</f>
+      <c r="I37" t="str">
+        <f t="shared" ref="I37:I38" si="64">VLOOKUP(A37,locations,2)</f>
         <v>Red Bull Ring - Spielberg</v>
       </c>
-      <c r="J33" t="str">
-        <f t="shared" ref="J33:J34" si="51">VLOOKUP(A33,locations,3)</f>
+      <c r="J37" t="str">
+        <f t="shared" ref="J37:J38" si="65">VLOOKUP(A37,locations,3)</f>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D34" t="str">
+      <c r="D38" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Vienna</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E38" s="4">
         <v>45157</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F38" s="6">
         <v>0.625</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G38" s="4">
         <f t="shared" si="45"/>
         <v>45157</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H38" s="6">
         <v>0.64583333333333337</v>
       </c>
-      <c r="I34" t="str">
-        <f t="shared" si="50"/>
+      <c r="I38" t="str">
+        <f t="shared" si="64"/>
         <v>Red Bull Ring - Spielberg</v>
       </c>
-      <c r="J34" t="str">
-        <f t="shared" si="51"/>
+      <c r="J38" t="str">
+        <f t="shared" si="65"/>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D35" t="str">
+      <c r="D39" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Vienna</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E39" s="4">
         <v>45158</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F39" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G39" s="4">
         <f t="shared" si="45"/>
         <v>45158</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H39" s="6">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I35" t="str">
-        <f t="shared" ref="I35" si="52">VLOOKUP(A35,locations,2)</f>
+      <c r="I39" t="str">
+        <f t="shared" ref="I39" si="66">VLOOKUP(A39,locations,2)</f>
         <v>Red Bull Ring - Spielberg</v>
       </c>
-      <c r="J35" t="str">
-        <f t="shared" ref="J35" si="53">VLOOKUP(A35,locations,3)</f>
+      <c r="J39" t="str">
+        <f t="shared" ref="J39" si="67">VLOOKUP(A39,locations,3)</f>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D36" t="str">
+      <c r="D40" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Madrid</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E40" s="4">
         <v>45171</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F40" s="6">
         <v>0.4513888888888889</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G40" s="4">
         <f t="shared" si="45"/>
         <v>45171</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H40" s="6">
         <v>0.47916666666666669</v>
       </c>
-      <c r="I36" t="str">
-        <f t="shared" ref="I36:I37" si="54">VLOOKUP(A36,locations,2)</f>
+      <c r="I40" t="str">
+        <f t="shared" ref="I40:I41" si="68">VLOOKUP(A40,locations,2)</f>
         <v>Circuit de Barcelona-Catalunya</v>
       </c>
-      <c r="J36" t="str">
-        <f t="shared" ref="J36:J37" si="55">VLOOKUP(A36,locations,3)</f>
+      <c r="J40" t="str">
+        <f t="shared" ref="J40:J41" si="69">VLOOKUP(A40,locations,3)</f>
         <v>Gran Premi Monster Energy de Catalunya</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="B41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D37" t="str">
+      <c r="D41" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Madrid</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E41" s="4">
         <v>45171</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F41" s="6">
         <v>0.625</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G41" s="4">
         <f t="shared" si="45"/>
         <v>45171</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H41" s="6">
         <v>0.64583333333333337</v>
       </c>
-      <c r="I37" t="str">
-        <f t="shared" si="54"/>
+      <c r="I41" t="str">
+        <f t="shared" si="68"/>
         <v>Circuit de Barcelona-Catalunya</v>
       </c>
-      <c r="J37" t="str">
-        <f t="shared" si="55"/>
+      <c r="J41" t="str">
+        <f t="shared" si="69"/>
         <v>Gran Premi Monster Energy de Catalunya</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="B42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D38" t="str">
+      <c r="D42" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Madrid</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E42" s="4">
         <v>45172</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F42" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G42" s="4">
         <f t="shared" si="45"/>
         <v>45172</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H42" s="6">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I38" t="str">
-        <f t="shared" ref="I38" si="56">VLOOKUP(A38,locations,2)</f>
+      <c r="I42" t="str">
+        <f t="shared" ref="I42" si="70">VLOOKUP(A42,locations,2)</f>
         <v>Circuit de Barcelona-Catalunya</v>
       </c>
-      <c r="J38" t="str">
-        <f t="shared" ref="J38" si="57">VLOOKUP(A38,locations,3)</f>
+      <c r="J42" t="str">
+        <f t="shared" ref="J42" si="71">VLOOKUP(A42,locations,3)</f>
         <v>Gran Premi Monster Energy de Catalunya</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D39" t="str">
+      <c r="D43" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Rome</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E43" s="4">
         <v>45178</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F43" s="6">
         <v>0.4513888888888889</v>
       </c>
-      <c r="G39" s="4">
-        <f t="shared" ref="G39:G41" si="58">E39</f>
+      <c r="G43" s="4">
+        <f t="shared" ref="G43:G45" si="72">E43</f>
         <v>45178</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H43" s="6">
         <v>0.47916666666666669</v>
       </c>
-      <c r="I39" t="str">
-        <f t="shared" ref="I39:I40" si="59">VLOOKUP(A39,locations,2)</f>
+      <c r="I43" t="str">
+        <f t="shared" ref="I43:I44" si="73">VLOOKUP(A43,locations,2)</f>
         <v>Misano World Circuit Marco Simoncelli</v>
       </c>
-      <c r="J39" t="str">
-        <f t="shared" ref="J39:J40" si="60">VLOOKUP(A39,locations,3)</f>
+      <c r="J43" t="str">
+        <f t="shared" ref="J43:J44" si="74">VLOOKUP(A43,locations,3)</f>
         <v>Gran Premio di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="B44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D40" t="str">
+      <c r="D44" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Rome</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E44" s="4">
         <v>45178</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F44" s="6">
         <v>0.625</v>
       </c>
-      <c r="G40" s="4">
-        <f t="shared" si="58"/>
+      <c r="G44" s="4">
+        <f t="shared" si="72"/>
         <v>45178</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H44" s="6">
         <v>0.64583333333333337</v>
       </c>
-      <c r="I40" t="str">
-        <f t="shared" si="59"/>
+      <c r="I44" t="str">
+        <f t="shared" si="73"/>
         <v>Misano World Circuit Marco Simoncelli</v>
       </c>
-      <c r="J40" t="str">
-        <f t="shared" si="60"/>
+      <c r="J44" t="str">
+        <f t="shared" si="74"/>
         <v>Gran Premio di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="B45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D41" t="str">
+      <c r="D45" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Rome</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E45" s="4">
         <v>45179</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F45" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G41" s="4">
-        <f t="shared" si="58"/>
+      <c r="G45" s="4">
+        <f t="shared" si="72"/>
         <v>45179</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H45" s="6">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I41" t="str">
-        <f t="shared" ref="I41" si="61">VLOOKUP(A41,locations,2)</f>
+      <c r="I45" t="str">
+        <f t="shared" ref="I45" si="75">VLOOKUP(A45,locations,2)</f>
         <v>Misano World Circuit Marco Simoncelli</v>
       </c>
-      <c r="J41" t="str">
-        <f t="shared" ref="J41:J45" si="62">VLOOKUP(A41,locations,3)</f>
+      <c r="J45" t="str">
+        <f t="shared" ref="J45:J49" si="76">VLOOKUP(A45,locations,3)</f>
         <v>Gran Premio di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D42" t="str">
+      <c r="D46" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Rome</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E46" s="4">
         <v>45180</v>
       </c>
-      <c r="F42" s="6"/>
-      <c r="G42" s="4">
-        <f t="shared" ref="G42" si="63">E42</f>
+      <c r="F46" s="6"/>
+      <c r="G46" s="4">
+        <f t="shared" ref="G46" si="77">E46</f>
         <v>45180</v>
       </c>
-      <c r="H42" s="6"/>
-      <c r="I42" t="str">
-        <f t="shared" ref="I42" si="64">VLOOKUP(A42,locations,2)</f>
+      <c r="H46" s="6"/>
+      <c r="I46" t="str">
+        <f t="shared" ref="I46" si="78">VLOOKUP(A46,locations,2)</f>
         <v>Misano World Circuit Marco Simoncelli</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J46" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>106</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" ref="D43:D64" si="65">VLOOKUP(A43,locations,4)</f>
-        <v>Asia/Kolkata</v>
-      </c>
-      <c r="E43" s="4">
-        <v>45192</v>
-      </c>
-      <c r="F43" s="6">
-        <v>0.4513888888888889</v>
-      </c>
-      <c r="G43" s="4">
-        <f t="shared" ref="G43:G45" si="66">E43</f>
-        <v>45192</v>
-      </c>
-      <c r="H43" s="6">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="I43" t="str">
-        <f t="shared" ref="I43:I45" si="67">VLOOKUP(A43,locations,2)</f>
-        <v>Buddh International Circuit</v>
-      </c>
-      <c r="J43" t="str">
-        <f t="shared" si="62"/>
-        <v>Grand Prix of India</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>106</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Kolkata</v>
-      </c>
-      <c r="E44" s="4">
-        <v>45192</v>
-      </c>
-      <c r="F44" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="G44" s="4">
-        <f t="shared" si="66"/>
-        <v>45192</v>
-      </c>
-      <c r="H44" s="6">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="I44" t="str">
-        <f t="shared" si="67"/>
-        <v>Buddh International Circuit</v>
-      </c>
-      <c r="J44" t="str">
-        <f t="shared" si="62"/>
-        <v>Grand Prix of India</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>106</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Kolkata</v>
-      </c>
-      <c r="E45" s="4">
-        <v>45193</v>
-      </c>
-      <c r="F45" s="6">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G45" s="4">
-        <f t="shared" si="66"/>
-        <v>45193</v>
-      </c>
-      <c r="H45" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I45" t="str">
-        <f t="shared" si="67"/>
-        <v>Buddh International Circuit</v>
-      </c>
-      <c r="J45" t="str">
-        <f t="shared" si="62"/>
-        <v>Grand Prix of India</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Tokyo</v>
-      </c>
-      <c r="E46" s="4">
-        <v>45199</v>
-      </c>
-      <c r="F46" s="6">
-        <v>0.4513888888888889</v>
-      </c>
-      <c r="G46" s="4">
-        <f t="shared" ref="G46:G48" si="68">E46</f>
-        <v>45199</v>
-      </c>
-      <c r="H46" s="6">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="I46" t="str">
-        <f t="shared" ref="I46:I47" si="69">VLOOKUP(A46,locations,2)</f>
-        <v>Mobility Resort Motegi</v>
-      </c>
-      <c r="J46" t="str">
-        <f t="shared" ref="J46:J47" si="70">VLOOKUP(A46,locations,3)</f>
-        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Tokyo</v>
+        <f t="shared" ref="D47:D68" si="79">VLOOKUP(A47,locations,4)</f>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E47" s="4">
-        <v>45199</v>
+        <v>45192</v>
       </c>
       <c r="F47" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G47" s="4">
-        <f t="shared" si="68"/>
-        <v>45199</v>
+        <f t="shared" ref="G47:G49" si="80">E47</f>
+        <v>45192</v>
       </c>
       <c r="H47" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="69"/>
-        <v>Mobility Resort Motegi</v>
+        <f t="shared" ref="I47:I49" si="81">VLOOKUP(A47,locations,2)</f>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="70"/>
-        <v>Motul Grand Prix of Japan</v>
+        <f t="shared" si="76"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Tokyo</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E48" s="4">
-        <v>45200</v>
+        <v>45192</v>
       </c>
       <c r="F48" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G48" s="4">
-        <f t="shared" si="68"/>
-        <v>45200</v>
+        <f t="shared" si="80"/>
+        <v>45192</v>
       </c>
       <c r="H48" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" ref="I48" si="71">VLOOKUP(A48,locations,2)</f>
-        <v>Mobility Resort Motegi</v>
+        <f t="shared" si="81"/>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" ref="J48" si="72">VLOOKUP(A48,locations,3)</f>
-        <v>Motul Grand Prix of Japan</v>
+        <f t="shared" si="76"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Jakarta</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E49" s="4">
-        <v>45213</v>
+        <v>45193</v>
       </c>
       <c r="F49" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G49" s="4">
-        <f t="shared" ref="G49:G51" si="73">E49</f>
-        <v>45213</v>
+        <f t="shared" si="80"/>
+        <v>45193</v>
       </c>
       <c r="H49" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" ref="I49:I50" si="74">VLOOKUP(A49,locations,2)</f>
-        <v>Mandalika International Street Circuit</v>
+        <f t="shared" si="81"/>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" ref="J49:J50" si="75">VLOOKUP(A49,locations,3)</f>
-        <v>Pertamina Grand Prix of Indonesia</v>
+        <f t="shared" si="76"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Jakarta</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E50" s="4">
-        <v>45213</v>
+        <v>45199</v>
       </c>
       <c r="F50" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G50" s="4">
-        <f t="shared" si="73"/>
-        <v>45213</v>
+        <f t="shared" ref="G50:G52" si="82">E50</f>
+        <v>45199</v>
       </c>
       <c r="H50" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="74"/>
-        <v>Mandalika International Street Circuit</v>
+        <f t="shared" ref="I50:I51" si="83">VLOOKUP(A50,locations,2)</f>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" si="75"/>
-        <v>Pertamina Grand Prix of Indonesia</v>
+        <f t="shared" ref="J50:J51" si="84">VLOOKUP(A50,locations,3)</f>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Jakarta</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E51" s="4">
-        <v>45214</v>
+        <v>45199</v>
       </c>
       <c r="F51" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G51" s="4">
-        <f t="shared" si="73"/>
-        <v>45214</v>
+        <f t="shared" si="82"/>
+        <v>45199</v>
       </c>
       <c r="H51" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" ref="I51" si="76">VLOOKUP(A51,locations,2)</f>
-        <v>Mandalika International Street Circuit</v>
+        <f t="shared" si="83"/>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" ref="J51" si="77">VLOOKUP(A51,locations,3)</f>
-        <v>Pertamina Grand Prix of Indonesia</v>
+        <f t="shared" si="84"/>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="65"/>
-        <v>Australia/Melbourne</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E52" s="4">
-        <v>45220</v>
+        <v>45200</v>
       </c>
       <c r="F52" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G52" s="4">
-        <f t="shared" ref="G52:G54" si="78">E52</f>
-        <v>45220</v>
+        <f t="shared" si="82"/>
+        <v>45200</v>
       </c>
       <c r="H52" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" ref="I52:I53" si="79">VLOOKUP(A52,locations,2)</f>
-        <v>Phillip Island</v>
+        <f t="shared" ref="I52" si="85">VLOOKUP(A52,locations,2)</f>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" ref="J52:J53" si="80">VLOOKUP(A52,locations,3)</f>
-        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
+        <f t="shared" ref="J52" si="86">VLOOKUP(A52,locations,3)</f>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="65"/>
-        <v>Australia/Melbourne</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Jakarta</v>
       </c>
       <c r="E53" s="4">
-        <v>45220</v>
+        <v>45213</v>
       </c>
       <c r="F53" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G53" s="4">
-        <f t="shared" si="78"/>
-        <v>45220</v>
+        <f t="shared" ref="G53:G55" si="87">E53</f>
+        <v>45213</v>
       </c>
       <c r="H53" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="79"/>
-        <v>Phillip Island</v>
+        <f t="shared" ref="I53:I54" si="88">VLOOKUP(A53,locations,2)</f>
+        <v>Mandalika International Street Circuit</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" si="80"/>
-        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
+        <f t="shared" ref="J53:J54" si="89">VLOOKUP(A53,locations,3)</f>
+        <v>Pertamina Grand Prix of Indonesia</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="65"/>
-        <v>Australia/Melbourne</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Jakarta</v>
       </c>
       <c r="E54" s="4">
-        <v>45221</v>
+        <v>45213</v>
       </c>
       <c r="F54" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G54" s="4">
-        <f t="shared" si="78"/>
-        <v>45221</v>
+        <f t="shared" si="87"/>
+        <v>45213</v>
       </c>
       <c r="H54" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" ref="I54" si="81">VLOOKUP(A54,locations,2)</f>
-        <v>Phillip Island</v>
+        <f t="shared" si="88"/>
+        <v>Mandalika International Street Circuit</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" ref="J54" si="82">VLOOKUP(A54,locations,3)</f>
-        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
+        <f t="shared" si="89"/>
+        <v>Pertamina Grand Prix of Indonesia</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Bangkok</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Jakarta</v>
       </c>
       <c r="E55" s="4">
-        <v>45227</v>
+        <v>45214</v>
       </c>
       <c r="F55" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G55" s="4">
-        <f t="shared" ref="G55:G57" si="83">E55</f>
-        <v>45227</v>
+        <f t="shared" si="87"/>
+        <v>45214</v>
       </c>
       <c r="H55" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" ref="I55:I56" si="84">VLOOKUP(A55,locations,2)</f>
-        <v>Chang International Circuit</v>
+        <f t="shared" ref="I55" si="90">VLOOKUP(A55,locations,2)</f>
+        <v>Mandalika International Street Circuit</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" ref="J55:J56" si="85">VLOOKUP(A55,locations,3)</f>
-        <v>OR Thailand Grand Prix</v>
+        <f t="shared" ref="J55" si="91">VLOOKUP(A55,locations,3)</f>
+        <v>Pertamina Grand Prix of Indonesia</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Bangkok</v>
+        <f t="shared" si="79"/>
+        <v>Australia/Melbourne</v>
       </c>
       <c r="E56" s="4">
-        <v>45227</v>
+        <v>45220</v>
       </c>
       <c r="F56" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G56" s="4">
-        <f t="shared" si="83"/>
-        <v>45227</v>
+        <f t="shared" ref="G56:G58" si="92">E56</f>
+        <v>45220</v>
       </c>
       <c r="H56" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="84"/>
-        <v>Chang International Circuit</v>
+        <f t="shared" ref="I56:I57" si="93">VLOOKUP(A56,locations,2)</f>
+        <v>Phillip Island</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="85"/>
-        <v>OR Thailand Grand Prix</v>
+        <f t="shared" ref="J56:J57" si="94">VLOOKUP(A56,locations,3)</f>
+        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Bangkok</v>
+        <f t="shared" si="79"/>
+        <v>Australia/Melbourne</v>
       </c>
       <c r="E57" s="4">
-        <v>45228</v>
+        <v>45220</v>
       </c>
       <c r="F57" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G57" s="4">
-        <f t="shared" si="83"/>
-        <v>45228</v>
+        <f t="shared" si="92"/>
+        <v>45220</v>
       </c>
       <c r="H57" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" ref="I57" si="86">VLOOKUP(A57,locations,2)</f>
-        <v>Chang International Circuit</v>
+        <f t="shared" si="93"/>
+        <v>Phillip Island</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" ref="J57" si="87">VLOOKUP(A57,locations,3)</f>
-        <v>OR Thailand Grand Prix</v>
+        <f t="shared" si="94"/>
+        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Kuala_Lumpur</v>
+        <f t="shared" si="79"/>
+        <v>Australia/Melbourne</v>
       </c>
       <c r="E58" s="4">
-        <v>45241</v>
+        <v>45221</v>
       </c>
       <c r="F58" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G58" s="4">
-        <f t="shared" ref="G58:G60" si="88">E58</f>
-        <v>45241</v>
+        <f t="shared" si="92"/>
+        <v>45221</v>
       </c>
       <c r="H58" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" ref="I58:I59" si="89">VLOOKUP(A58,locations,2)</f>
-        <v>Sepang International Circuit</v>
+        <f t="shared" ref="I58" si="95">VLOOKUP(A58,locations,2)</f>
+        <v>Phillip Island</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" ref="J58:J59" si="90">VLOOKUP(A58,locations,3)</f>
-        <v>PETRONAS Grand Prix of Malaysia</v>
+        <f t="shared" ref="J58" si="96">VLOOKUP(A58,locations,3)</f>
+        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Kuala_Lumpur</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Bangkok</v>
       </c>
       <c r="E59" s="4">
-        <v>45241</v>
+        <v>45227</v>
       </c>
       <c r="F59" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G59" s="4">
-        <f t="shared" si="88"/>
-        <v>45241</v>
+        <f t="shared" ref="G59:G61" si="97">E59</f>
+        <v>45227</v>
       </c>
       <c r="H59" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="89"/>
-        <v>Sepang International Circuit</v>
+        <f t="shared" ref="I59:I60" si="98">VLOOKUP(A59,locations,2)</f>
+        <v>Chang International Circuit</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="90"/>
-        <v>PETRONAS Grand Prix of Malaysia</v>
+        <f t="shared" ref="J59:J60" si="99">VLOOKUP(A59,locations,3)</f>
+        <v>OR Thailand Grand Prix</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Kuala_Lumpur</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Bangkok</v>
       </c>
       <c r="E60" s="4">
-        <v>45242</v>
+        <v>45227</v>
       </c>
       <c r="F60" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G60" s="4">
-        <f t="shared" si="88"/>
-        <v>45242</v>
+        <f t="shared" si="97"/>
+        <v>45227</v>
       </c>
       <c r="H60" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" ref="I60" si="91">VLOOKUP(A60,locations,2)</f>
-        <v>Sepang International Circuit</v>
+        <f t="shared" si="98"/>
+        <v>Chang International Circuit</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" ref="J60" si="92">VLOOKUP(A60,locations,3)</f>
-        <v>PETRONAS Grand Prix of Malaysia</v>
+        <f t="shared" si="99"/>
+        <v>OR Thailand Grand Prix</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Qatar</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Bangkok</v>
       </c>
       <c r="E61" s="4">
-        <v>45248</v>
+        <v>45228</v>
       </c>
       <c r="F61" s="6">
-        <v>0.65972222222222221</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G61" s="4">
-        <f>E61</f>
-        <v>45248</v>
+        <f t="shared" si="97"/>
+        <v>45228</v>
       </c>
       <c r="H61" s="6">
-        <v>0.6875</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" ref="I61:I62" si="93">VLOOKUP(A61,locations,2)</f>
-        <v>Losail International Circuit</v>
+        <f t="shared" ref="I61" si="100">VLOOKUP(A61,locations,2)</f>
+        <v>Chang International Circuit</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" ref="J61:J62" si="94">VLOOKUP(A61,locations,3)</f>
-        <v>Grand Prix of Qatar</v>
+        <f t="shared" ref="J61" si="101">VLOOKUP(A61,locations,3)</f>
+        <v>OR Thailand Grand Prix</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Qatar</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Kuala_Lumpur</v>
       </c>
       <c r="E62" s="4">
-        <v>45248</v>
+        <v>45241</v>
       </c>
       <c r="F62" s="6">
-        <v>0.83333333333333337</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G62" s="4">
-        <f>E62</f>
-        <v>45248</v>
+        <f t="shared" ref="G62:G64" si="102">E62</f>
+        <v>45241</v>
       </c>
       <c r="H62" s="6">
-        <v>0.85416666666666663</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="93"/>
-        <v>Losail International Circuit</v>
+        <f t="shared" ref="I62:I63" si="103">VLOOKUP(A62,locations,2)</f>
+        <v>Sepang International Circuit</v>
       </c>
       <c r="J62" t="str">
-        <f t="shared" si="94"/>
-        <v>Grand Prix of Qatar</v>
+        <f t="shared" ref="J62:J63" si="104">VLOOKUP(A62,locations,3)</f>
+        <v>PETRONAS Grand Prix of Malaysia</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="65"/>
-        <v>Asia/Qatar</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Kuala_Lumpur</v>
       </c>
       <c r="E63" s="4">
-        <v>45249</v>
+        <v>45241</v>
       </c>
       <c r="F63" s="6">
-        <v>0.83333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G63" s="4">
-        <f>E63</f>
-        <v>45249</v>
+        <f t="shared" si="102"/>
+        <v>45241</v>
       </c>
       <c r="H63" s="6">
-        <v>0.86805555555555547</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" ref="I63" si="95">VLOOKUP(A63,locations,2)</f>
-        <v>Losail International Circuit</v>
+        <f t="shared" si="103"/>
+        <v>Sepang International Circuit</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" ref="J63" si="96">VLOOKUP(A63,locations,3)</f>
-        <v>Grand Prix of Qatar</v>
+        <f t="shared" si="104"/>
+        <v>PETRONAS Grand Prix of Malaysia</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" si="65"/>
-        <v>Europe/Madrid</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Kuala_Lumpur</v>
       </c>
       <c r="E64" s="4">
-        <v>45255</v>
+        <v>45242</v>
       </c>
       <c r="F64" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G64" s="4">
-        <f t="shared" ref="G64:G66" si="97">E64</f>
-        <v>45255</v>
+        <f t="shared" si="102"/>
+        <v>45242</v>
       </c>
       <c r="H64" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" ref="I64:I65" si="98">VLOOKUP(A64,locations,2)</f>
-        <v>Circuit Ricardo Tormo</v>
+        <f t="shared" ref="I64" si="105">VLOOKUP(A64,locations,2)</f>
+        <v>Sepang International Circuit</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" ref="J64:J65" si="99">VLOOKUP(A64,locations,3)</f>
-        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+        <f t="shared" ref="J64" si="106">VLOOKUP(A64,locations,3)</f>
+        <v>PETRONAS Grand Prix of Malaysia</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" ref="D65" si="100">VLOOKUP(A65,locations,4)</f>
-        <v>Europe/Madrid</v>
+        <f t="shared" si="79"/>
+        <v>Asia/Qatar</v>
       </c>
       <c r="E65" s="4">
-        <v>45255</v>
+        <v>45248</v>
       </c>
       <c r="F65" s="6">
-        <v>0.625</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="G65" s="4">
-        <f t="shared" si="97"/>
-        <v>45255</v>
+        <f>E65</f>
+        <v>45248</v>
       </c>
       <c r="H65" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="98"/>
-        <v>Circuit Ricardo Tormo</v>
+        <f t="shared" ref="I65:I66" si="107">VLOOKUP(A65,locations,2)</f>
+        <v>Losail International Circuit</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" si="99"/>
-        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+        <f t="shared" ref="J65:J66" si="108">VLOOKUP(A65,locations,3)</f>
+        <v>Grand Prix of Qatar</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="79"/>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E66" s="4">
+        <v>45248</v>
+      </c>
+      <c r="F66" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G66" s="4">
+        <f>E66</f>
+        <v>45248</v>
+      </c>
+      <c r="H66" s="6">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="107"/>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="108"/>
+        <v>Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="79"/>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E67" s="4">
+        <v>45249</v>
+      </c>
+      <c r="F67" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G67" s="4">
+        <f>E67</f>
+        <v>45249</v>
+      </c>
+      <c r="H67" s="6">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" ref="I67" si="109">VLOOKUP(A67,locations,2)</f>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" ref="J67" si="110">VLOOKUP(A67,locations,3)</f>
+        <v>Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>37</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="3" t="s">
+      <c r="B68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="79"/>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E68" s="4">
+        <v>45255</v>
+      </c>
+      <c r="F68" s="6">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G68" s="4">
+        <f t="shared" ref="G68:G70" si="111">E68</f>
+        <v>45255</v>
+      </c>
+      <c r="H68" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" ref="I68:I69" si="112">VLOOKUP(A68,locations,2)</f>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" ref="J68:J69" si="113">VLOOKUP(A68,locations,3)</f>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>37</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" ref="D69" si="114">VLOOKUP(A69,locations,4)</f>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E69" s="4">
+        <v>45255</v>
+      </c>
+      <c r="F69" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G69" s="4">
+        <f t="shared" si="111"/>
+        <v>45255</v>
+      </c>
+      <c r="H69" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="112"/>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="113"/>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>37</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D66" t="str">
-        <f t="shared" ref="D66" si="101">VLOOKUP(A66,locations,4)</f>
+      <c r="D70" t="str">
+        <f t="shared" ref="D70" si="115">VLOOKUP(A70,locations,4)</f>
         <v>Europe/Madrid</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E70" s="4">
         <v>45256</v>
       </c>
-      <c r="F66" s="6">
+      <c r="F70" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G66" s="4">
-        <f t="shared" si="97"/>
+      <c r="G70" s="4">
+        <f t="shared" si="111"/>
         <v>45256</v>
       </c>
-      <c r="H66" s="6">
+      <c r="H70" s="6">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I66" t="str">
-        <f t="shared" ref="I66" si="102">VLOOKUP(A66,locations,2)</f>
+      <c r="I70" t="str">
+        <f t="shared" ref="I70" si="116">VLOOKUP(A70,locations,2)</f>
         <v>Circuit Ricardo Tormo</v>
       </c>
-      <c r="J66" t="str">
-        <f t="shared" ref="J66" si="103">VLOOKUP(A66,locations,3)</f>
+      <c r="J70" t="str">
+        <f t="shared" ref="J70" si="117">VLOOKUP(A70,locations,3)</f>
         <v>Gran Premio Motul de la Comunitat Valenciana</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A71:A74 A2:A66" xr:uid="{F03BE25C-DA6F-6246-A9E5-DB905318EDFD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A75:A78 A2:A70" xr:uid="{F03BE25C-DA6F-6246-A9E5-DB905318EDFD}">
       <formula1>countries</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71:B74 B2:B66" xr:uid="{0EA54380-98F5-E141-93FA-55C8FE75E20E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75:B78 B2:B70" xr:uid="{0EA54380-98F5-E141-93FA-55C8FE75E20E}">
       <formula1>categories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C71:C74 C2:C66" xr:uid="{8F2CDCBC-21D9-4843-9F7D-D70F3A2F785B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C75:C78 C2:C70" xr:uid="{8F2CDCBC-21D9-4843-9F7D-D70F3A2F785B}">
       <formula1>sessions</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add Moto3 and Moto2 qualifying and races for AT
</commit_message>
<xml_diff>
--- a/motogp/MotoGP.xlsx
+++ b/motogp/MotoGP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/motogp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8BF9758-9F3B-8C41-A618-F7F5D903A373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{614232C2-4B21-724A-B521-ECCC93F5CDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="1900" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="117">
   <si>
     <t>Country</t>
   </si>
@@ -776,7 +776,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A264AA3C-A8BA-6F48-8FC0-C3E78D3BD742}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1251,7 +1251,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" ref="D14:D46" si="22">VLOOKUP(A14,locations,4)</f>
+        <f t="shared" ref="D14:D50" si="22">VLOOKUP(A14,locations,4)</f>
         <v>Europe/Madrid</v>
       </c>
       <c r="E14" s="4">
@@ -1832,7 +1832,7 @@
         <v>0.4513888888888889</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" ref="G30:G42" si="45">E30</f>
+        <f t="shared" ref="G30:G46" si="45">E30</f>
         <v>45143</v>
       </c>
       <c r="H30" s="6">
@@ -2091,11 +2091,11 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" ref="I37:I38" si="64">VLOOKUP(A37,locations,2)</f>
+        <f t="shared" ref="I37:I40" si="64">VLOOKUP(A37,locations,2)</f>
         <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" ref="J37:J38" si="65">VLOOKUP(A37,locations,3)</f>
+        <f t="shared" ref="J37:J40" si="65">VLOOKUP(A37,locations,3)</f>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
@@ -2104,10 +2104,10 @@
         <v>30</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="22"/>
@@ -2117,21 +2117,21 @@
         <v>45157</v>
       </c>
       <c r="F38" s="6">
-        <v>0.625</v>
+        <v>0.53472222222222221</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="45"/>
         <v>45157</v>
       </c>
       <c r="H38" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" ref="I38:I39" si="66">VLOOKUP(A38,locations,2)</f>
         <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" ref="J38:J39" si="67">VLOOKUP(A38,locations,3)</f>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
@@ -2140,287 +2140,292 @@
         <v>30</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Vienna</v>
       </c>
       <c r="E39" s="4">
-        <v>45158</v>
+        <v>45157</v>
       </c>
       <c r="F39" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="45"/>
-        <v>45158</v>
+        <v>45157</v>
       </c>
       <c r="H39" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" ref="I39" si="66">VLOOKUP(A39,locations,2)</f>
+        <f t="shared" si="66"/>
         <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" ref="J39" si="67">VLOOKUP(A39,locations,3)</f>
+        <f t="shared" si="67"/>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="22"/>
-        <v>Europe/Madrid</v>
+        <v>Europe/Vienna</v>
       </c>
       <c r="E40" s="4">
-        <v>45171</v>
+        <v>45157</v>
       </c>
       <c r="F40" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.625</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="45"/>
-        <v>45171</v>
+        <v>45157</v>
       </c>
       <c r="H40" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" ref="I40:I41" si="68">VLOOKUP(A40,locations,2)</f>
-        <v>Circuit de Barcelona-Catalunya</v>
+        <f t="shared" si="64"/>
+        <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" ref="J40:J41" si="69">VLOOKUP(A40,locations,3)</f>
-        <v>Gran Premi Monster Energy de Catalunya</v>
+        <f t="shared" si="65"/>
+        <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="22"/>
-        <v>Europe/Madrid</v>
+        <v>Europe/Vienna</v>
       </c>
       <c r="E41" s="4">
-        <v>45171</v>
+        <v>45158</v>
       </c>
       <c r="F41" s="6">
-        <v>0.625</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="45"/>
-        <v>45171</v>
+        <v>45158</v>
       </c>
       <c r="H41" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="68"/>
-        <v>Circuit de Barcelona-Catalunya</v>
+        <f t="shared" ref="I41:I42" si="68">VLOOKUP(A41,locations,2)</f>
+        <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" si="69"/>
-        <v>Gran Premi Monster Energy de Catalunya</v>
+        <f t="shared" ref="J41:J42" si="69">VLOOKUP(A41,locations,3)</f>
+        <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="22"/>
-        <v>Europe/Madrid</v>
+        <v>Europe/Vienna</v>
       </c>
       <c r="E42" s="4">
-        <v>45172</v>
+        <v>45158</v>
       </c>
       <c r="F42" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="45"/>
-        <v>45172</v>
+        <v>45158</v>
       </c>
       <c r="H42" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.55902777777777779</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" ref="I42" si="70">VLOOKUP(A42,locations,2)</f>
-        <v>Circuit de Barcelona-Catalunya</v>
+        <f t="shared" si="68"/>
+        <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" ref="J42" si="71">VLOOKUP(A42,locations,3)</f>
-        <v>Gran Premi Monster Energy de Catalunya</v>
+        <f t="shared" si="69"/>
+        <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="22"/>
-        <v>Europe/Rome</v>
+        <v>Europe/Vienna</v>
       </c>
       <c r="E43" s="4">
-        <v>45178</v>
+        <v>45158</v>
       </c>
       <c r="F43" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G43" s="4">
-        <f t="shared" ref="G43:G45" si="72">E43</f>
-        <v>45178</v>
+        <f t="shared" si="45"/>
+        <v>45158</v>
       </c>
       <c r="H43" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" ref="I43:I44" si="73">VLOOKUP(A43,locations,2)</f>
-        <v>Misano World Circuit Marco Simoncelli</v>
+        <f t="shared" ref="I43" si="70">VLOOKUP(A43,locations,2)</f>
+        <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" ref="J43:J44" si="74">VLOOKUP(A43,locations,3)</f>
-        <v>Gran Premio di San Marino e della Riviera di Rimini</v>
+        <f t="shared" ref="J43" si="71">VLOOKUP(A43,locations,3)</f>
+        <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="22"/>
-        <v>Europe/Rome</v>
+        <v>Europe/Madrid</v>
       </c>
       <c r="E44" s="4">
-        <v>45178</v>
+        <v>45171</v>
       </c>
       <c r="F44" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G44" s="4">
-        <f t="shared" si="72"/>
-        <v>45178</v>
+        <f t="shared" si="45"/>
+        <v>45171</v>
       </c>
       <c r="H44" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="73"/>
-        <v>Misano World Circuit Marco Simoncelli</v>
+        <f t="shared" ref="I44:I45" si="72">VLOOKUP(A44,locations,2)</f>
+        <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" si="74"/>
-        <v>Gran Premio di San Marino e della Riviera di Rimini</v>
+        <f t="shared" ref="J44:J45" si="73">VLOOKUP(A44,locations,3)</f>
+        <v>Gran Premi Monster Energy de Catalunya</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="22"/>
-        <v>Europe/Rome</v>
+        <v>Europe/Madrid</v>
       </c>
       <c r="E45" s="4">
-        <v>45179</v>
+        <v>45171</v>
       </c>
       <c r="F45" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G45" s="4">
+        <f t="shared" si="45"/>
+        <v>45171</v>
+      </c>
+      <c r="H45" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I45" t="str">
         <f t="shared" si="72"/>
-        <v>45179</v>
-      </c>
-      <c r="H45" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I45" t="str">
-        <f t="shared" ref="I45" si="75">VLOOKUP(A45,locations,2)</f>
-        <v>Misano World Circuit Marco Simoncelli</v>
+        <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" ref="J45:J49" si="76">VLOOKUP(A45,locations,3)</f>
-        <v>Gran Premio di San Marino e della Riviera di Rimini</v>
+        <f t="shared" si="73"/>
+        <v>Gran Premi Monster Energy de Catalunya</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="22"/>
-        <v>Europe/Rome</v>
+        <v>Europe/Madrid</v>
       </c>
       <c r="E46" s="4">
-        <v>45180</v>
-      </c>
-      <c r="F46" s="6"/>
+        <v>45172</v>
+      </c>
+      <c r="F46" s="6">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G46" s="4">
-        <f t="shared" ref="G46" si="77">E46</f>
-        <v>45180</v>
-      </c>
-      <c r="H46" s="6"/>
+        <f t="shared" si="45"/>
+        <v>45172</v>
+      </c>
+      <c r="H46" s="6">
+        <v>0.61805555555555558</v>
+      </c>
       <c r="I46" t="str">
-        <f t="shared" ref="I46" si="78">VLOOKUP(A46,locations,2)</f>
-        <v>Misano World Circuit Marco Simoncelli</v>
-      </c>
-      <c r="J46" t="s">
-        <v>105</v>
+        <f t="shared" ref="I46" si="74">VLOOKUP(A46,locations,2)</f>
+        <v>Circuit de Barcelona-Catalunya</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" ref="J46" si="75">VLOOKUP(A46,locations,3)</f>
+        <v>Gran Premi Monster Energy de Catalunya</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>12</v>
@@ -2429,34 +2434,34 @@
         <v>16</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" ref="D47:D68" si="79">VLOOKUP(A47,locations,4)</f>
-        <v>Asia/Kolkata</v>
+        <f t="shared" si="22"/>
+        <v>Europe/Rome</v>
       </c>
       <c r="E47" s="4">
-        <v>45192</v>
+        <v>45178</v>
       </c>
       <c r="F47" s="6">
         <v>0.4513888888888889</v>
       </c>
       <c r="G47" s="4">
-        <f t="shared" ref="G47:G49" si="80">E47</f>
-        <v>45192</v>
+        <f t="shared" ref="G47:G49" si="76">E47</f>
+        <v>45178</v>
       </c>
       <c r="H47" s="6">
         <v>0.47916666666666669</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" ref="I47:I49" si="81">VLOOKUP(A47,locations,2)</f>
-        <v>Buddh International Circuit</v>
+        <f t="shared" ref="I47:I48" si="77">VLOOKUP(A47,locations,2)</f>
+        <v>Misano World Circuit Marco Simoncelli</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="76"/>
-        <v>Grand Prix of India</v>
+        <f t="shared" ref="J47:J48" si="78">VLOOKUP(A47,locations,3)</f>
+        <v>Gran Premio di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -2465,34 +2470,34 @@
         <v>90</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Kolkata</v>
+        <f t="shared" si="22"/>
+        <v>Europe/Rome</v>
       </c>
       <c r="E48" s="4">
-        <v>45192</v>
+        <v>45178</v>
       </c>
       <c r="F48" s="6">
         <v>0.625</v>
       </c>
       <c r="G48" s="4">
-        <f t="shared" si="80"/>
-        <v>45192</v>
+        <f t="shared" si="76"/>
+        <v>45178</v>
       </c>
       <c r="H48" s="6">
         <v>0.64583333333333337</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="81"/>
-        <v>Buddh International Circuit</v>
+        <f t="shared" si="77"/>
+        <v>Misano World Circuit Marco Simoncelli</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="76"/>
-        <v>Grand Prix of India</v>
+        <f t="shared" si="78"/>
+        <v>Gran Premio di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>12</v>
@@ -2501,797 +2506,936 @@
         <v>15</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Kolkata</v>
+        <f t="shared" si="22"/>
+        <v>Europe/Rome</v>
       </c>
       <c r="E49" s="4">
-        <v>45193</v>
+        <v>45179</v>
       </c>
       <c r="F49" s="6">
         <v>0.58333333333333337</v>
       </c>
       <c r="G49" s="4">
-        <f t="shared" si="80"/>
-        <v>45193</v>
+        <f t="shared" si="76"/>
+        <v>45179</v>
       </c>
       <c r="H49" s="6">
         <v>0.61805555555555558</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="81"/>
-        <v>Buddh International Circuit</v>
+        <f t="shared" ref="I49" si="79">VLOOKUP(A49,locations,2)</f>
+        <v>Misano World Circuit Marco Simoncelli</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" si="76"/>
-        <v>Grand Prix of India</v>
+        <f t="shared" ref="J49:J53" si="80">VLOOKUP(A49,locations,3)</f>
+        <v>Gran Premio di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Tokyo</v>
+        <f t="shared" si="22"/>
+        <v>Europe/Rome</v>
       </c>
       <c r="E50" s="4">
-        <v>45199</v>
-      </c>
-      <c r="F50" s="6">
-        <v>0.4513888888888889</v>
-      </c>
+        <v>45180</v>
+      </c>
+      <c r="F50" s="6"/>
       <c r="G50" s="4">
-        <f t="shared" ref="G50:G52" si="82">E50</f>
-        <v>45199</v>
-      </c>
-      <c r="H50" s="6">
-        <v>0.47916666666666669</v>
-      </c>
+        <f t="shared" ref="G50" si="81">E50</f>
+        <v>45180</v>
+      </c>
+      <c r="H50" s="6"/>
       <c r="I50" t="str">
-        <f t="shared" ref="I50:I51" si="83">VLOOKUP(A50,locations,2)</f>
-        <v>Mobility Resort Motegi</v>
-      </c>
-      <c r="J50" t="str">
-        <f t="shared" ref="J50:J51" si="84">VLOOKUP(A50,locations,3)</f>
-        <v>Motul Grand Prix of Japan</v>
+        <f t="shared" ref="I50" si="82">VLOOKUP(A50,locations,2)</f>
+        <v>Misano World Circuit Marco Simoncelli</v>
+      </c>
+      <c r="J50" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Tokyo</v>
+        <f t="shared" ref="D51:D72" si="83">VLOOKUP(A51,locations,4)</f>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E51" s="4">
-        <v>45199</v>
+        <v>45192</v>
       </c>
       <c r="F51" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G51" s="4">
-        <f t="shared" si="82"/>
-        <v>45199</v>
+        <f t="shared" ref="G51:G53" si="84">E51</f>
+        <v>45192</v>
       </c>
       <c r="H51" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="83"/>
-        <v>Mobility Resort Motegi</v>
+        <f t="shared" ref="I51:I53" si="85">VLOOKUP(A51,locations,2)</f>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" si="84"/>
-        <v>Motul Grand Prix of Japan</v>
+        <f t="shared" si="80"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Tokyo</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E52" s="4">
-        <v>45200</v>
+        <v>45192</v>
       </c>
       <c r="F52" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G52" s="4">
-        <f t="shared" si="82"/>
-        <v>45200</v>
+        <f t="shared" si="84"/>
+        <v>45192</v>
       </c>
       <c r="H52" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" ref="I52" si="85">VLOOKUP(A52,locations,2)</f>
-        <v>Mobility Resort Motegi</v>
+        <f t="shared" si="85"/>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" ref="J52" si="86">VLOOKUP(A52,locations,3)</f>
-        <v>Motul Grand Prix of Japan</v>
+        <f t="shared" si="80"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Jakarta</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E53" s="4">
-        <v>45213</v>
+        <v>45193</v>
       </c>
       <c r="F53" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G53" s="4">
-        <f t="shared" ref="G53:G55" si="87">E53</f>
-        <v>45213</v>
+        <f t="shared" si="84"/>
+        <v>45193</v>
       </c>
       <c r="H53" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" ref="I53:I54" si="88">VLOOKUP(A53,locations,2)</f>
-        <v>Mandalika International Street Circuit</v>
+        <f t="shared" si="85"/>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" ref="J53:J54" si="89">VLOOKUP(A53,locations,3)</f>
-        <v>Pertamina Grand Prix of Indonesia</v>
+        <f t="shared" si="80"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Jakarta</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E54" s="4">
-        <v>45213</v>
+        <v>45199</v>
       </c>
       <c r="F54" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G54" s="4">
-        <f t="shared" si="87"/>
-        <v>45213</v>
+        <f t="shared" ref="G54:G56" si="86">E54</f>
+        <v>45199</v>
       </c>
       <c r="H54" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="88"/>
-        <v>Mandalika International Street Circuit</v>
+        <f t="shared" ref="I54:I55" si="87">VLOOKUP(A54,locations,2)</f>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" si="89"/>
-        <v>Pertamina Grand Prix of Indonesia</v>
+        <f t="shared" ref="J54:J55" si="88">VLOOKUP(A54,locations,3)</f>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Jakarta</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E55" s="4">
-        <v>45214</v>
+        <v>45199</v>
       </c>
       <c r="F55" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G55" s="4">
+        <f t="shared" si="86"/>
+        <v>45199</v>
+      </c>
+      <c r="H55" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I55" t="str">
         <f t="shared" si="87"/>
-        <v>45214</v>
-      </c>
-      <c r="H55" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I55" t="str">
-        <f t="shared" ref="I55" si="90">VLOOKUP(A55,locations,2)</f>
-        <v>Mandalika International Street Circuit</v>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" ref="J55" si="91">VLOOKUP(A55,locations,3)</f>
-        <v>Pertamina Grand Prix of Indonesia</v>
+        <f t="shared" si="88"/>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="79"/>
-        <v>Australia/Melbourne</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E56" s="4">
-        <v>45220</v>
+        <v>45200</v>
       </c>
       <c r="F56" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G56" s="4">
-        <f t="shared" ref="G56:G58" si="92">E56</f>
-        <v>45220</v>
+        <f t="shared" si="86"/>
+        <v>45200</v>
       </c>
       <c r="H56" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" ref="I56:I57" si="93">VLOOKUP(A56,locations,2)</f>
-        <v>Phillip Island</v>
+        <f t="shared" ref="I56" si="89">VLOOKUP(A56,locations,2)</f>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" ref="J56:J57" si="94">VLOOKUP(A56,locations,3)</f>
-        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
+        <f t="shared" ref="J56" si="90">VLOOKUP(A56,locations,3)</f>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="79"/>
-        <v>Australia/Melbourne</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Jakarta</v>
       </c>
       <c r="E57" s="4">
-        <v>45220</v>
+        <v>45213</v>
       </c>
       <c r="F57" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G57" s="4">
-        <f t="shared" si="92"/>
-        <v>45220</v>
+        <f t="shared" ref="G57:G59" si="91">E57</f>
+        <v>45213</v>
       </c>
       <c r="H57" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="93"/>
-        <v>Phillip Island</v>
+        <f t="shared" ref="I57:I58" si="92">VLOOKUP(A57,locations,2)</f>
+        <v>Mandalika International Street Circuit</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" si="94"/>
-        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
+        <f t="shared" ref="J57:J58" si="93">VLOOKUP(A57,locations,3)</f>
+        <v>Pertamina Grand Prix of Indonesia</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="79"/>
-        <v>Australia/Melbourne</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Jakarta</v>
       </c>
       <c r="E58" s="4">
-        <v>45221</v>
+        <v>45213</v>
       </c>
       <c r="F58" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G58" s="4">
+        <f t="shared" si="91"/>
+        <v>45213</v>
+      </c>
+      <c r="H58" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I58" t="str">
         <f t="shared" si="92"/>
-        <v>45221</v>
-      </c>
-      <c r="H58" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I58" t="str">
-        <f t="shared" ref="I58" si="95">VLOOKUP(A58,locations,2)</f>
-        <v>Phillip Island</v>
+        <v>Mandalika International Street Circuit</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" ref="J58" si="96">VLOOKUP(A58,locations,3)</f>
-        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
+        <f t="shared" si="93"/>
+        <v>Pertamina Grand Prix of Indonesia</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Bangkok</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Jakarta</v>
       </c>
       <c r="E59" s="4">
-        <v>45227</v>
+        <v>45214</v>
       </c>
       <c r="F59" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G59" s="4">
-        <f t="shared" ref="G59:G61" si="97">E59</f>
-        <v>45227</v>
+        <f t="shared" si="91"/>
+        <v>45214</v>
       </c>
       <c r="H59" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" ref="I59:I60" si="98">VLOOKUP(A59,locations,2)</f>
-        <v>Chang International Circuit</v>
+        <f t="shared" ref="I59" si="94">VLOOKUP(A59,locations,2)</f>
+        <v>Mandalika International Street Circuit</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" ref="J59:J60" si="99">VLOOKUP(A59,locations,3)</f>
-        <v>OR Thailand Grand Prix</v>
+        <f t="shared" ref="J59" si="95">VLOOKUP(A59,locations,3)</f>
+        <v>Pertamina Grand Prix of Indonesia</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Bangkok</v>
+        <f t="shared" si="83"/>
+        <v>Australia/Melbourne</v>
       </c>
       <c r="E60" s="4">
-        <v>45227</v>
+        <v>45220</v>
       </c>
       <c r="F60" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G60" s="4">
-        <f t="shared" si="97"/>
-        <v>45227</v>
+        <f t="shared" ref="G60:G62" si="96">E60</f>
+        <v>45220</v>
       </c>
       <c r="H60" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="98"/>
-        <v>Chang International Circuit</v>
+        <f t="shared" ref="I60:I61" si="97">VLOOKUP(A60,locations,2)</f>
+        <v>Phillip Island</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="99"/>
-        <v>OR Thailand Grand Prix</v>
+        <f t="shared" ref="J60:J61" si="98">VLOOKUP(A60,locations,3)</f>
+        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Bangkok</v>
+        <f t="shared" si="83"/>
+        <v>Australia/Melbourne</v>
       </c>
       <c r="E61" s="4">
-        <v>45228</v>
+        <v>45220</v>
       </c>
       <c r="F61" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G61" s="4">
+        <f t="shared" si="96"/>
+        <v>45220</v>
+      </c>
+      <c r="H61" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I61" t="str">
         <f t="shared" si="97"/>
-        <v>45228</v>
-      </c>
-      <c r="H61" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I61" t="str">
-        <f t="shared" ref="I61" si="100">VLOOKUP(A61,locations,2)</f>
-        <v>Chang International Circuit</v>
+        <v>Phillip Island</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" ref="J61" si="101">VLOOKUP(A61,locations,3)</f>
-        <v>OR Thailand Grand Prix</v>
+        <f t="shared" si="98"/>
+        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Kuala_Lumpur</v>
+        <f t="shared" si="83"/>
+        <v>Australia/Melbourne</v>
       </c>
       <c r="E62" s="4">
-        <v>45241</v>
+        <v>45221</v>
       </c>
       <c r="F62" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G62" s="4">
-        <f t="shared" ref="G62:G64" si="102">E62</f>
-        <v>45241</v>
+        <f t="shared" si="96"/>
+        <v>45221</v>
       </c>
       <c r="H62" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" ref="I62:I63" si="103">VLOOKUP(A62,locations,2)</f>
-        <v>Sepang International Circuit</v>
+        <f t="shared" ref="I62" si="99">VLOOKUP(A62,locations,2)</f>
+        <v>Phillip Island</v>
       </c>
       <c r="J62" t="str">
-        <f t="shared" ref="J62:J63" si="104">VLOOKUP(A62,locations,3)</f>
-        <v>PETRONAS Grand Prix of Malaysia</v>
+        <f t="shared" ref="J62" si="100">VLOOKUP(A62,locations,3)</f>
+        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Kuala_Lumpur</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Bangkok</v>
       </c>
       <c r="E63" s="4">
-        <v>45241</v>
+        <v>45227</v>
       </c>
       <c r="F63" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G63" s="4">
-        <f t="shared" si="102"/>
-        <v>45241</v>
+        <f t="shared" ref="G63:G65" si="101">E63</f>
+        <v>45227</v>
       </c>
       <c r="H63" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="103"/>
-        <v>Sepang International Circuit</v>
+        <f t="shared" ref="I63:I64" si="102">VLOOKUP(A63,locations,2)</f>
+        <v>Chang International Circuit</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" si="104"/>
-        <v>PETRONAS Grand Prix of Malaysia</v>
+        <f t="shared" ref="J63:J64" si="103">VLOOKUP(A63,locations,3)</f>
+        <v>OR Thailand Grand Prix</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Kuala_Lumpur</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Bangkok</v>
       </c>
       <c r="E64" s="4">
-        <v>45242</v>
+        <v>45227</v>
       </c>
       <c r="F64" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G64" s="4">
+        <f t="shared" si="101"/>
+        <v>45227</v>
+      </c>
+      <c r="H64" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I64" t="str">
         <f t="shared" si="102"/>
-        <v>45242</v>
-      </c>
-      <c r="H64" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I64" t="str">
-        <f t="shared" ref="I64" si="105">VLOOKUP(A64,locations,2)</f>
-        <v>Sepang International Circuit</v>
+        <v>Chang International Circuit</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" ref="J64" si="106">VLOOKUP(A64,locations,3)</f>
-        <v>PETRONAS Grand Prix of Malaysia</v>
+        <f t="shared" si="103"/>
+        <v>OR Thailand Grand Prix</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Qatar</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Bangkok</v>
       </c>
       <c r="E65" s="4">
-        <v>45248</v>
+        <v>45228</v>
       </c>
       <c r="F65" s="6">
-        <v>0.65972222222222221</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G65" s="4">
-        <f>E65</f>
-        <v>45248</v>
+        <f t="shared" si="101"/>
+        <v>45228</v>
       </c>
       <c r="H65" s="6">
-        <v>0.6875</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" ref="I65:I66" si="107">VLOOKUP(A65,locations,2)</f>
-        <v>Losail International Circuit</v>
+        <f t="shared" ref="I65" si="104">VLOOKUP(A65,locations,2)</f>
+        <v>Chang International Circuit</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" ref="J65:J66" si="108">VLOOKUP(A65,locations,3)</f>
-        <v>Grand Prix of Qatar</v>
+        <f t="shared" ref="J65" si="105">VLOOKUP(A65,locations,3)</f>
+        <v>OR Thailand Grand Prix</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Qatar</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Kuala_Lumpur</v>
       </c>
       <c r="E66" s="4">
-        <v>45248</v>
+        <v>45241</v>
       </c>
       <c r="F66" s="6">
-        <v>0.83333333333333337</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G66" s="4">
-        <f>E66</f>
-        <v>45248</v>
+        <f t="shared" ref="G66:G68" si="106">E66</f>
+        <v>45241</v>
       </c>
       <c r="H66" s="6">
-        <v>0.85416666666666663</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="107"/>
-        <v>Losail International Circuit</v>
+        <f t="shared" ref="I66:I67" si="107">VLOOKUP(A66,locations,2)</f>
+        <v>Sepang International Circuit</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" si="108"/>
-        <v>Grand Prix of Qatar</v>
+        <f t="shared" ref="J66:J67" si="108">VLOOKUP(A66,locations,3)</f>
+        <v>PETRONAS Grand Prix of Malaysia</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" si="79"/>
-        <v>Asia/Qatar</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Kuala_Lumpur</v>
       </c>
       <c r="E67" s="4">
-        <v>45249</v>
+        <v>45241</v>
       </c>
       <c r="F67" s="6">
-        <v>0.83333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G67" s="4">
-        <f>E67</f>
-        <v>45249</v>
+        <f t="shared" si="106"/>
+        <v>45241</v>
       </c>
       <c r="H67" s="6">
-        <v>0.86805555555555547</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67" si="109">VLOOKUP(A67,locations,2)</f>
-        <v>Losail International Circuit</v>
+        <f t="shared" si="107"/>
+        <v>Sepang International Circuit</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67" si="110">VLOOKUP(A67,locations,3)</f>
-        <v>Grand Prix of Qatar</v>
+        <f t="shared" si="108"/>
+        <v>PETRONAS Grand Prix of Malaysia</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="79"/>
-        <v>Europe/Madrid</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Kuala_Lumpur</v>
       </c>
       <c r="E68" s="4">
-        <v>45255</v>
+        <v>45242</v>
       </c>
       <c r="F68" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G68" s="4">
-        <f t="shared" ref="G68:G70" si="111">E68</f>
-        <v>45255</v>
+        <f t="shared" si="106"/>
+        <v>45242</v>
       </c>
       <c r="H68" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" ref="I68:I69" si="112">VLOOKUP(A68,locations,2)</f>
-        <v>Circuit Ricardo Tormo</v>
+        <f t="shared" ref="I68" si="109">VLOOKUP(A68,locations,2)</f>
+        <v>Sepang International Circuit</v>
       </c>
       <c r="J68" t="str">
-        <f t="shared" ref="J68:J69" si="113">VLOOKUP(A68,locations,3)</f>
-        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+        <f t="shared" ref="J68" si="110">VLOOKUP(A68,locations,3)</f>
+        <v>PETRONAS Grand Prix of Malaysia</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" ref="D69" si="114">VLOOKUP(A69,locations,4)</f>
-        <v>Europe/Madrid</v>
+        <f t="shared" si="83"/>
+        <v>Asia/Qatar</v>
       </c>
       <c r="E69" s="4">
-        <v>45255</v>
+        <v>45248</v>
       </c>
       <c r="F69" s="6">
-        <v>0.625</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="G69" s="4">
-        <f t="shared" si="111"/>
-        <v>45255</v>
+        <f>E69</f>
+        <v>45248</v>
       </c>
       <c r="H69" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="112"/>
-        <v>Circuit Ricardo Tormo</v>
+        <f t="shared" ref="I69:I70" si="111">VLOOKUP(A69,locations,2)</f>
+        <v>Losail International Circuit</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" si="113"/>
-        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+        <f t="shared" ref="J69:J70" si="112">VLOOKUP(A69,locations,3)</f>
+        <v>Grand Prix of Qatar</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="83"/>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E70" s="4">
+        <v>45248</v>
+      </c>
+      <c r="F70" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G70" s="4">
+        <f>E70</f>
+        <v>45248</v>
+      </c>
+      <c r="H70" s="6">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" si="111"/>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="112"/>
+        <v>Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="83"/>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E71" s="4">
+        <v>45249</v>
+      </c>
+      <c r="F71" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G71" s="4">
+        <f>E71</f>
+        <v>45249</v>
+      </c>
+      <c r="H71" s="6">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" ref="I71" si="113">VLOOKUP(A71,locations,2)</f>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" ref="J71" si="114">VLOOKUP(A71,locations,3)</f>
+        <v>Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>37</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C70" s="3" t="s">
+      <c r="B72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="83"/>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E72" s="4">
+        <v>45255</v>
+      </c>
+      <c r="F72" s="6">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G72" s="4">
+        <f t="shared" ref="G72:G74" si="115">E72</f>
+        <v>45255</v>
+      </c>
+      <c r="H72" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" ref="I72:I73" si="116">VLOOKUP(A72,locations,2)</f>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" ref="J72:J73" si="117">VLOOKUP(A72,locations,3)</f>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>37</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" ref="D73" si="118">VLOOKUP(A73,locations,4)</f>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E73" s="4">
+        <v>45255</v>
+      </c>
+      <c r="F73" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G73" s="4">
+        <f t="shared" si="115"/>
+        <v>45255</v>
+      </c>
+      <c r="H73" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I73" t="str">
+        <f t="shared" si="116"/>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="117"/>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>37</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D70" t="str">
-        <f t="shared" ref="D70" si="115">VLOOKUP(A70,locations,4)</f>
+      <c r="D74" t="str">
+        <f t="shared" ref="D74" si="119">VLOOKUP(A74,locations,4)</f>
         <v>Europe/Madrid</v>
       </c>
-      <c r="E70" s="4">
+      <c r="E74" s="4">
         <v>45256</v>
       </c>
-      <c r="F70" s="6">
+      <c r="F74" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G70" s="4">
-        <f t="shared" si="111"/>
+      <c r="G74" s="4">
+        <f t="shared" si="115"/>
         <v>45256</v>
       </c>
-      <c r="H70" s="6">
+      <c r="H74" s="6">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I70" t="str">
-        <f t="shared" ref="I70" si="116">VLOOKUP(A70,locations,2)</f>
+      <c r="I74" t="str">
+        <f t="shared" ref="I74" si="120">VLOOKUP(A74,locations,2)</f>
         <v>Circuit Ricardo Tormo</v>
       </c>
-      <c r="J70" t="str">
-        <f t="shared" ref="J70" si="117">VLOOKUP(A70,locations,3)</f>
+      <c r="J74" t="str">
+        <f t="shared" ref="J74" si="121">VLOOKUP(A74,locations,3)</f>
         <v>Gran Premio Motul de la Comunitat Valenciana</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A75:A78 A2:A70" xr:uid="{F03BE25C-DA6F-6246-A9E5-DB905318EDFD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A79:A82 A2:A74" xr:uid="{F03BE25C-DA6F-6246-A9E5-DB905318EDFD}">
       <formula1>countries</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75:B78 B2:B70" xr:uid="{0EA54380-98F5-E141-93FA-55C8FE75E20E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79:B82 B2:B74" xr:uid="{0EA54380-98F5-E141-93FA-55C8FE75E20E}">
       <formula1>categories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C75:C78 C2:C70" xr:uid="{8F2CDCBC-21D9-4843-9F7D-D70F3A2F785B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C79:C82 C2:C74" xr:uid="{8F2CDCBC-21D9-4843-9F7D-D70F3A2F785B}">
       <formula1>sessions</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add temporary Excel files
</commit_message>
<xml_diff>
--- a/motogp/MotoGP.xlsx
+++ b/motogp/MotoGP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/motogp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{614232C2-4B21-724A-B521-ECCC93F5CDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FC5A61-4890-7A46-9C06-8F1FCE9CCB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="1900" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -778,7 +778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A264AA3C-A8BA-6F48-8FC0-C3E78D3BD742}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Add Moto2 and Moto3 for all remaining races
</commit_message>
<xml_diff>
--- a/motogp/MotoGP.xlsx
+++ b/motogp/MotoGP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/motogp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FC5A61-4890-7A46-9C06-8F1FCE9CCB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0235E8C-7FC5-1F4F-9E3D-53D5C67D4411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="1900" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
+    <workbookView xWindow="3560" yWindow="1900" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
   <sheets>
     <sheet name="MotoGP" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="118">
   <si>
     <t>Country</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Titles</t>
   </si>
   <si>
-    <t>Grand Prix of Qatar</t>
-  </si>
-  <si>
     <t>Asia/Qatar</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>Misano World Circuit Marco Simoncelli</t>
   </si>
   <si>
-    <t>Gran Premio di San Marino e della Riviera di Rimini</t>
-  </si>
-  <si>
     <t>MotorLand Aragón</t>
   </si>
   <si>
@@ -316,9 +310,6 @@
     <t>Portimao MotoGP Official Test</t>
   </si>
   <si>
-    <t>Sprint Race</t>
-  </si>
-  <si>
     <t>Gran Premio Michelin de la República Argentina</t>
   </si>
   <si>
@@ -385,9 +376,6 @@
     <t>Pertamina Grand Prix of Indonesia</t>
   </si>
   <si>
-    <t>Animoca Brands Australian Motorcycle Grand Prix</t>
-  </si>
-  <si>
     <t>OR Thailand Grand Prix</t>
   </si>
   <si>
@@ -395,6 +383,21 @@
   </si>
   <si>
     <t>Gran Premio Motul de la Comunitat Valenciana</t>
+  </si>
+  <si>
+    <t>Silverstone Moto2 and Moto3 Offical Test</t>
+  </si>
+  <si>
+    <t>Gran Premio Red Bull di San Marino e della Riviera di Rimini</t>
+  </si>
+  <si>
+    <t>MotoGP Guru by Gryfyn Australian Motorcycle Grand Prix</t>
+  </si>
+  <si>
+    <t>Tissot Sprint</t>
+  </si>
+  <si>
+    <t>Qatar Airways Grand Prix of Qatar</t>
   </si>
 </sst>
 </file>
@@ -776,23 +779,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A264AA3C-A8BA-6F48-8FC0-C3E78D3BD742}">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.83203125" style="3"/>
     <col min="7" max="7" width="10.83203125" style="4"/>
     <col min="8" max="8" width="10.83203125" style="3"/>
     <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -836,7 +837,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2" si="0">VLOOKUP(A2,locations,4)</f>
@@ -855,7 +856,7 @@
         <v>Sepang International Circuit</v>
       </c>
       <c r="J2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -866,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3" si="2">VLOOKUP(A3,locations,4)</f>
@@ -885,7 +886,7 @@
         <v>Sepang International Circuit</v>
       </c>
       <c r="J3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -896,7 +897,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4" si="4">VLOOKUP(A4,locations,4)</f>
@@ -915,7 +916,7 @@
         <v>Autódromo Internacional do Algarve</v>
       </c>
       <c r="J4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -962,7 +963,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="6"/>
@@ -1070,7 +1071,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D9" t="str">
         <f>VLOOKUP(A9,locations,4)</f>
@@ -1178,7 +1179,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="16"/>
@@ -1253,7 +1254,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" ref="D14:D50" si="22">VLOOKUP(A14,locations,4)</f>
+        <f t="shared" ref="D14:D59" si="22">VLOOKUP(A14,locations,4)</f>
         <v>Europe/Madrid</v>
       </c>
       <c r="E14" s="4">
@@ -1286,7 +1287,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="22"/>
@@ -1358,7 +1359,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="22"/>
@@ -1378,7 +1379,7 @@
         <v>Circuito de Jerez - Angel Nieto</v>
       </c>
       <c r="J17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1425,7 +1426,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="22"/>
@@ -1533,7 +1534,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="22"/>
@@ -1641,7 +1642,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="22"/>
@@ -1749,7 +1750,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="22"/>
@@ -1834,7 +1835,7 @@
         <v>0.4513888888888889</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" ref="G30:G46" si="45">E30</f>
+        <f t="shared" ref="G30:G51" si="45">E30</f>
         <v>45143</v>
       </c>
       <c r="H30" s="6">
@@ -1929,7 +1930,7 @@
         <v>12</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="22"/>
@@ -2040,7 +2041,7 @@
         <v>15</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" ref="D36" si="60">VLOOKUP(A36,locations,4)</f>
+        <f t="shared" ref="D36:D37" si="60">VLOOKUP(A36,locations,4)</f>
         <v>Europe/London</v>
       </c>
       <c r="E36" s="4">
@@ -2050,14 +2051,14 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="G36" s="4">
-        <f t="shared" ref="G36" si="61">E36</f>
+        <f t="shared" ref="G36:G37" si="61">E36</f>
         <v>45144</v>
       </c>
       <c r="H36" s="6">
         <v>0.63194444444444442</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" ref="I36" si="62">VLOOKUP(A36,locations,2)</f>
+        <f t="shared" ref="I36:I37" si="62">VLOOKUP(A36,locations,2)</f>
         <v>Silverstone</v>
       </c>
       <c r="J36" t="str">
@@ -2067,38 +2068,33 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="22"/>
-        <v>Europe/Vienna</v>
+        <f t="shared" si="60"/>
+        <v>Europe/London</v>
       </c>
       <c r="E37" s="4">
-        <v>45157</v>
-      </c>
-      <c r="F37" s="6">
-        <v>0.4513888888888889</v>
-      </c>
+        <v>45145</v>
+      </c>
+      <c r="F37" s="6"/>
       <c r="G37" s="4">
-        <f t="shared" si="45"/>
-        <v>45157</v>
-      </c>
-      <c r="H37" s="6">
-        <v>0.47916666666666669</v>
-      </c>
+        <f t="shared" si="61"/>
+        <v>45145</v>
+      </c>
+      <c r="H37" s="6"/>
       <c r="I37" t="str">
-        <f t="shared" ref="I37:I40" si="64">VLOOKUP(A37,locations,2)</f>
-        <v>Red Bull Ring - Spielberg</v>
-      </c>
-      <c r="J37" t="str">
-        <f t="shared" ref="J37:J40" si="65">VLOOKUP(A37,locations,3)</f>
-        <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
+        <f t="shared" si="62"/>
+        <v>Silverstone</v>
+      </c>
+      <c r="J37" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -2106,7 +2102,7 @@
         <v>30</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>16</v>
@@ -2119,21 +2115,21 @@
         <v>45157</v>
       </c>
       <c r="F38" s="6">
-        <v>0.53472222222222221</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="45"/>
         <v>45157</v>
       </c>
       <c r="H38" s="6">
-        <v>0.5625</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" ref="I38:I39" si="66">VLOOKUP(A38,locations,2)</f>
+        <f t="shared" ref="I38:I41" si="64">VLOOKUP(A38,locations,2)</f>
         <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" ref="J38:J39" si="67">VLOOKUP(A38,locations,3)</f>
+        <f t="shared" ref="J38:J41" si="65">VLOOKUP(A38,locations,3)</f>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
@@ -2142,7 +2138,7 @@
         <v>30</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>16</v>
@@ -2155,21 +2151,21 @@
         <v>45157</v>
       </c>
       <c r="F39" s="6">
-        <v>0.57291666666666663</v>
+        <v>0.53472222222222221</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="45"/>
         <v>45157</v>
       </c>
       <c r="H39" s="6">
-        <v>0.60069444444444442</v>
+        <v>0.5625</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" ref="I39:I40" si="66">VLOOKUP(A39,locations,2)</f>
         <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" ref="J39:J40" si="67">VLOOKUP(A39,locations,3)</f>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
@@ -2178,10 +2174,10 @@
         <v>30</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="22"/>
@@ -2191,21 +2187,21 @@
         <v>45157</v>
       </c>
       <c r="F40" s="6">
-        <v>0.625</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="45"/>
         <v>45157</v>
       </c>
       <c r="H40" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
@@ -2214,34 +2210,34 @@
         <v>30</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Vienna</v>
       </c>
       <c r="E41" s="4">
-        <v>45158</v>
+        <v>45157</v>
       </c>
       <c r="F41" s="6">
-        <v>0.45833333333333331</v>
+        <v>0.625</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="45"/>
-        <v>45158</v>
+        <v>45157</v>
       </c>
       <c r="H41" s="6">
-        <v>0.4861111111111111</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" ref="I41:I42" si="68">VLOOKUP(A41,locations,2)</f>
+        <f t="shared" si="64"/>
         <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" ref="J41:J42" si="69">VLOOKUP(A41,locations,3)</f>
+        <f t="shared" si="65"/>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
@@ -2250,7 +2246,7 @@
         <v>30</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>15</v>
@@ -2263,21 +2259,21 @@
         <v>45158</v>
       </c>
       <c r="F42" s="6">
-        <v>0.51041666666666663</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="45"/>
         <v>45158</v>
       </c>
       <c r="H42" s="6">
-        <v>0.55902777777777779</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" ref="I42:I43" si="68">VLOOKUP(A42,locations,2)</f>
         <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" ref="J42:J43" si="69">VLOOKUP(A42,locations,3)</f>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
@@ -2286,7 +2282,7 @@
         <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>15</v>
@@ -2299,58 +2295,58 @@
         <v>45158</v>
       </c>
       <c r="F43" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" si="45"/>
         <v>45158</v>
       </c>
       <c r="H43" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.55902777777777779</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" ref="I43" si="70">VLOOKUP(A43,locations,2)</f>
+        <f t="shared" si="68"/>
         <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" ref="J43" si="71">VLOOKUP(A43,locations,3)</f>
+        <f t="shared" si="69"/>
         <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="22"/>
-        <v>Europe/Madrid</v>
+        <v>Europe/Vienna</v>
       </c>
       <c r="E44" s="4">
-        <v>45171</v>
+        <v>45158</v>
       </c>
       <c r="F44" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="45"/>
-        <v>45171</v>
+        <v>45158</v>
       </c>
       <c r="H44" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" ref="I44:I45" si="72">VLOOKUP(A44,locations,2)</f>
-        <v>Circuit de Barcelona-Catalunya</v>
+        <f t="shared" ref="I44" si="70">VLOOKUP(A44,locations,2)</f>
+        <v>Red Bull Ring - Spielberg</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" ref="J44:J45" si="73">VLOOKUP(A44,locations,3)</f>
-        <v>Gran Premi Monster Energy de Catalunya</v>
+        <f t="shared" ref="J44" si="71">VLOOKUP(A44,locations,3)</f>
+        <v>CryptoDATA Motorrad Grand Prix von Österreich</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -2361,7 +2357,7 @@
         <v>12</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="22"/>
@@ -2371,21 +2367,21 @@
         <v>45171</v>
       </c>
       <c r="F45" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="45"/>
         <v>45171</v>
       </c>
       <c r="H45" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="72"/>
+        <f t="shared" ref="I45:I48" si="72">VLOOKUP(A45,locations,2)</f>
         <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" si="73"/>
+        <f t="shared" ref="J45:J48" si="73">VLOOKUP(A45,locations,3)</f>
         <v>Gran Premi Monster Energy de Catalunya</v>
       </c>
     </row>
@@ -2394,503 +2390,503 @@
         <v>25</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D46" t="str">
+        <f t="shared" ref="D46:D47" si="74">VLOOKUP(A46,locations,4)</f>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E46" s="4">
+        <v>45171</v>
+      </c>
+      <c r="F46" s="6">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="G46" s="4">
+        <f t="shared" si="45"/>
+        <v>45171</v>
+      </c>
+      <c r="H46" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" ref="I46:I47" si="75">VLOOKUP(A46,locations,2)</f>
+        <v>Circuit de Barcelona-Catalunya</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" ref="J46:J47" si="76">VLOOKUP(A46,locations,3)</f>
+        <v>Gran Premi Monster Energy de Catalunya</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="74"/>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E47" s="4">
+        <v>45171</v>
+      </c>
+      <c r="F47" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G47" s="4">
+        <f t="shared" si="45"/>
+        <v>45171</v>
+      </c>
+      <c r="H47" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="75"/>
+        <v>Circuit de Barcelona-Catalunya</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="76"/>
+        <v>Gran Premi Monster Energy de Catalunya</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Madrid</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E48" s="4">
+        <v>45171</v>
+      </c>
+      <c r="F48" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G48" s="4">
+        <f t="shared" si="45"/>
+        <v>45171</v>
+      </c>
+      <c r="H48" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="72"/>
+        <v>Circuit de Barcelona-Catalunya</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="73"/>
+        <v>Gran Premi Monster Energy de Catalunya</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" ref="D49:D50" si="77">VLOOKUP(A49,locations,4)</f>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E49" s="4">
         <v>45172</v>
       </c>
-      <c r="F46" s="6">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G46" s="4">
+      <c r="F49" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G49" s="4">
         <f t="shared" si="45"/>
         <v>45172</v>
       </c>
-      <c r="H46" s="6">
+      <c r="H49" s="6">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" ref="I49:I50" si="78">VLOOKUP(A49,locations,2)</f>
+        <v>Circuit de Barcelona-Catalunya</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" ref="J49:J50" si="79">VLOOKUP(A49,locations,3)</f>
+        <v>Gran Premi Monster Energy de Catalunya</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="77"/>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E50" s="4">
+        <v>45172</v>
+      </c>
+      <c r="F50" s="6">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G50" s="4">
+        <f t="shared" si="45"/>
+        <v>45172</v>
+      </c>
+      <c r="H50" s="6">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="78"/>
+        <v>Circuit de Barcelona-Catalunya</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="79"/>
+        <v>Gran Premi Monster Energy de Catalunya</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="22"/>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E51" s="4">
+        <v>45172</v>
+      </c>
+      <c r="F51" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G51" s="4">
+        <f t="shared" si="45"/>
+        <v>45172</v>
+      </c>
+      <c r="H51" s="6">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I46" t="str">
-        <f t="shared" ref="I46" si="74">VLOOKUP(A46,locations,2)</f>
+      <c r="I51" t="str">
+        <f t="shared" ref="I51" si="80">VLOOKUP(A51,locations,2)</f>
         <v>Circuit de Barcelona-Catalunya</v>
       </c>
-      <c r="J46" t="str">
-        <f t="shared" ref="J46" si="75">VLOOKUP(A46,locations,3)</f>
+      <c r="J51" t="str">
+        <f t="shared" ref="J51" si="81">VLOOKUP(A51,locations,3)</f>
         <v>Gran Premi Monster Energy de Catalunya</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="B52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D47" t="str">
+      <c r="D52" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Rome</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E52" s="4">
         <v>45178</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F52" s="6">
         <v>0.4513888888888889</v>
       </c>
-      <c r="G47" s="4">
-        <f t="shared" ref="G47:G49" si="76">E47</f>
+      <c r="G52" s="4">
+        <f t="shared" ref="G52:G58" si="82">E52</f>
         <v>45178</v>
       </c>
-      <c r="H47" s="6">
+      <c r="H52" s="6">
         <v>0.47916666666666669</v>
       </c>
-      <c r="I47" t="str">
-        <f t="shared" ref="I47:I48" si="77">VLOOKUP(A47,locations,2)</f>
+      <c r="I52" t="str">
+        <f t="shared" ref="I52:I55" si="83">VLOOKUP(A52,locations,2)</f>
         <v>Misano World Circuit Marco Simoncelli</v>
       </c>
-      <c r="J47" t="str">
-        <f t="shared" ref="J47:J48" si="78">VLOOKUP(A47,locations,3)</f>
-        <v>Gran Premio di San Marino e della Riviera di Rimini</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="J52" t="str">
+        <f t="shared" ref="J52:J55" si="84">VLOOKUP(A52,locations,3)</f>
+        <v>Gran Premio Red Bull di San Marino e della Riviera di Rimini</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D48" t="str">
+      <c r="B53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Rome</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E53" s="4">
         <v>45178</v>
       </c>
-      <c r="F48" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="G48" s="4">
-        <f t="shared" si="76"/>
+      <c r="F53" s="6">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="G53" s="4">
+        <f t="shared" si="82"/>
         <v>45178</v>
       </c>
-      <c r="H48" s="6">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="I48" t="str">
-        <f t="shared" si="77"/>
+      <c r="H53" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" ref="I53:I54" si="85">VLOOKUP(A53,locations,2)</f>
         <v>Misano World Circuit Marco Simoncelli</v>
       </c>
-      <c r="J48" t="str">
-        <f t="shared" si="78"/>
-        <v>Gran Premio di San Marino e della Riviera di Rimini</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="J53" t="str">
+        <f t="shared" ref="J53:J54" si="86">VLOOKUP(A53,locations,3)</f>
+        <v>Gran Premio Red Bull di San Marino e della Riviera di Rimini</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" t="str">
+      <c r="B54" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Rome</v>
       </c>
-      <c r="E49" s="4">
-        <v>45179</v>
-      </c>
-      <c r="F49" s="6">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G49" s="4">
-        <f t="shared" si="76"/>
-        <v>45179</v>
-      </c>
-      <c r="H49" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I49" t="str">
-        <f t="shared" ref="I49" si="79">VLOOKUP(A49,locations,2)</f>
+      <c r="E54" s="4">
+        <v>45178</v>
+      </c>
+      <c r="F54" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G54" s="4">
+        <f t="shared" si="82"/>
+        <v>45178</v>
+      </c>
+      <c r="H54" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="85"/>
         <v>Misano World Circuit Marco Simoncelli</v>
       </c>
-      <c r="J49" t="str">
-        <f t="shared" ref="J49:J53" si="80">VLOOKUP(A49,locations,3)</f>
-        <v>Gran Premio di San Marino e della Riviera di Rimini</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="J54" t="str">
+        <f t="shared" si="86"/>
+        <v>Gran Premio Red Bull di San Marino e della Riviera di Rimini</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D50" t="str">
+      <c r="B55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" t="str">
         <f t="shared" si="22"/>
         <v>Europe/Rome</v>
       </c>
-      <c r="E50" s="4">
-        <v>45180</v>
-      </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="4">
-        <f t="shared" ref="G50" si="81">E50</f>
-        <v>45180</v>
-      </c>
-      <c r="H50" s="6"/>
-      <c r="I50" t="str">
-        <f t="shared" ref="I50" si="82">VLOOKUP(A50,locations,2)</f>
-        <v>Misano World Circuit Marco Simoncelli</v>
-      </c>
-      <c r="J50" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>106</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" t="str">
-        <f t="shared" ref="D51:D72" si="83">VLOOKUP(A51,locations,4)</f>
-        <v>Asia/Kolkata</v>
-      </c>
-      <c r="E51" s="4">
-        <v>45192</v>
-      </c>
-      <c r="F51" s="6">
-        <v>0.4513888888888889</v>
-      </c>
-      <c r="G51" s="4">
-        <f t="shared" ref="G51:G53" si="84">E51</f>
-        <v>45192</v>
-      </c>
-      <c r="H51" s="6">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="I51" t="str">
-        <f t="shared" ref="I51:I53" si="85">VLOOKUP(A51,locations,2)</f>
-        <v>Buddh International Circuit</v>
-      </c>
-      <c r="J51" t="str">
-        <f t="shared" si="80"/>
-        <v>Grand Prix of India</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Kolkata</v>
-      </c>
-      <c r="E52" s="4">
-        <v>45192</v>
-      </c>
-      <c r="F52" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="G52" s="4">
-        <f t="shared" si="84"/>
-        <v>45192</v>
-      </c>
-      <c r="H52" s="6">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="I52" t="str">
-        <f t="shared" si="85"/>
-        <v>Buddh International Circuit</v>
-      </c>
-      <c r="J52" t="str">
-        <f t="shared" si="80"/>
-        <v>Grand Prix of India</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>106</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D53" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Kolkata</v>
-      </c>
-      <c r="E53" s="4">
-        <v>45193</v>
-      </c>
-      <c r="F53" s="6">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G53" s="4">
-        <f t="shared" si="84"/>
-        <v>45193</v>
-      </c>
-      <c r="H53" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I53" t="str">
-        <f t="shared" si="85"/>
-        <v>Buddh International Circuit</v>
-      </c>
-      <c r="J53" t="str">
-        <f t="shared" si="80"/>
-        <v>Grand Prix of India</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>33</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Tokyo</v>
-      </c>
-      <c r="E54" s="4">
-        <v>45199</v>
-      </c>
-      <c r="F54" s="6">
-        <v>0.4513888888888889</v>
-      </c>
-      <c r="G54" s="4">
-        <f t="shared" ref="G54:G56" si="86">E54</f>
-        <v>45199</v>
-      </c>
-      <c r="H54" s="6">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="I54" t="str">
-        <f t="shared" ref="I54:I55" si="87">VLOOKUP(A54,locations,2)</f>
-        <v>Mobility Resort Motegi</v>
-      </c>
-      <c r="J54" t="str">
-        <f t="shared" ref="J54:J55" si="88">VLOOKUP(A54,locations,3)</f>
-        <v>Motul Grand Prix of Japan</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>33</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Tokyo</v>
-      </c>
       <c r="E55" s="4">
-        <v>45199</v>
+        <v>45178</v>
       </c>
       <c r="F55" s="6">
         <v>0.625</v>
       </c>
       <c r="G55" s="4">
-        <f t="shared" si="86"/>
-        <v>45199</v>
+        <f t="shared" si="82"/>
+        <v>45178</v>
       </c>
       <c r="H55" s="6">
         <v>0.64583333333333337</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="87"/>
-        <v>Mobility Resort Motegi</v>
+        <f t="shared" si="83"/>
+        <v>Misano World Circuit Marco Simoncelli</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="88"/>
-        <v>Motul Grand Prix of Japan</v>
+        <f t="shared" si="84"/>
+        <v>Gran Premio Red Bull di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Tokyo</v>
+        <f t="shared" ref="D56:D57" si="87">VLOOKUP(A56,locations,4)</f>
+        <v>Europe/Rome</v>
       </c>
       <c r="E56" s="4">
-        <v>45200</v>
+        <v>45179</v>
       </c>
       <c r="F56" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="G56" s="4">
-        <f t="shared" si="86"/>
-        <v>45200</v>
+        <f t="shared" si="82"/>
+        <v>45179</v>
       </c>
       <c r="H56" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" ref="I56" si="89">VLOOKUP(A56,locations,2)</f>
-        <v>Mobility Resort Motegi</v>
+        <f t="shared" ref="I56:I57" si="88">VLOOKUP(A56,locations,2)</f>
+        <v>Misano World Circuit Marco Simoncelli</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" ref="J56" si="90">VLOOKUP(A56,locations,3)</f>
-        <v>Motul Grand Prix of Japan</v>
+        <f t="shared" ref="J56:J57" si="89">VLOOKUP(A56,locations,3)</f>
+        <v>Gran Premio Red Bull di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Jakarta</v>
+        <f t="shared" si="87"/>
+        <v>Europe/Rome</v>
       </c>
       <c r="E57" s="4">
-        <v>45213</v>
+        <v>45179</v>
       </c>
       <c r="F57" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="G57" s="4">
-        <f t="shared" ref="G57:G59" si="91">E57</f>
-        <v>45213</v>
+        <f t="shared" si="82"/>
+        <v>45179</v>
       </c>
       <c r="H57" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.55902777777777779</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" ref="I57:I58" si="92">VLOOKUP(A57,locations,2)</f>
-        <v>Mandalika International Street Circuit</v>
+        <f t="shared" si="88"/>
+        <v>Misano World Circuit Marco Simoncelli</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" ref="J57:J58" si="93">VLOOKUP(A57,locations,3)</f>
-        <v>Pertamina Grand Prix of Indonesia</v>
+        <f t="shared" si="89"/>
+        <v>Gran Premio Red Bull di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Jakarta</v>
+        <f t="shared" si="22"/>
+        <v>Europe/Rome</v>
       </c>
       <c r="E58" s="4">
-        <v>45213</v>
+        <v>45179</v>
       </c>
       <c r="F58" s="6">
-        <v>0.625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G58" s="4">
-        <f t="shared" si="91"/>
-        <v>45213</v>
+        <f t="shared" si="82"/>
+        <v>45179</v>
       </c>
       <c r="H58" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="92"/>
-        <v>Mandalika International Street Circuit</v>
+        <f t="shared" ref="I58" si="90">VLOOKUP(A58,locations,2)</f>
+        <v>Misano World Circuit Marco Simoncelli</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="93"/>
-        <v>Pertamina Grand Prix of Indonesia</v>
+        <f t="shared" ref="J58:J66" si="91">VLOOKUP(A58,locations,3)</f>
+        <v>Gran Premio Red Bull di San Marino e della Riviera di Rimini</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Jakarta</v>
+        <f t="shared" si="22"/>
+        <v>Europe/Rome</v>
       </c>
       <c r="E59" s="4">
-        <v>45214</v>
-      </c>
-      <c r="F59" s="6">
-        <v>0.58333333333333337</v>
-      </c>
+        <v>45180</v>
+      </c>
+      <c r="F59" s="6"/>
       <c r="G59" s="4">
-        <f t="shared" si="91"/>
-        <v>45214</v>
-      </c>
-      <c r="H59" s="6">
-        <v>0.61805555555555558</v>
-      </c>
+        <f t="shared" ref="G59" si="92">E59</f>
+        <v>45180</v>
+      </c>
+      <c r="H59" s="6"/>
       <c r="I59" t="str">
-        <f t="shared" ref="I59" si="94">VLOOKUP(A59,locations,2)</f>
-        <v>Mandalika International Street Circuit</v>
-      </c>
-      <c r="J59" t="str">
-        <f t="shared" ref="J59" si="95">VLOOKUP(A59,locations,3)</f>
-        <v>Pertamina Grand Prix of Indonesia</v>
+        <f t="shared" ref="I59" si="93">VLOOKUP(A59,locations,2)</f>
+        <v>Misano World Circuit Marco Simoncelli</v>
+      </c>
+      <c r="J59" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>12</v>
@@ -2899,545 +2895,2021 @@
         <v>16</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="83"/>
-        <v>Australia/Melbourne</v>
+        <f t="shared" ref="D60:D111" si="94">VLOOKUP(A60,locations,4)</f>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E60" s="4">
-        <v>45220</v>
+        <v>45192</v>
       </c>
       <c r="F60" s="6">
         <v>0.4513888888888889</v>
       </c>
       <c r="G60" s="4">
-        <f t="shared" ref="G60:G62" si="96">E60</f>
-        <v>45220</v>
+        <f t="shared" ref="G60:G66" si="95">E60</f>
+        <v>45192</v>
       </c>
       <c r="H60" s="6">
         <v>0.47916666666666669</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" ref="I60:I61" si="97">VLOOKUP(A60,locations,2)</f>
-        <v>Phillip Island</v>
+        <f t="shared" ref="I60:I66" si="96">VLOOKUP(A60,locations,2)</f>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" ref="J60:J61" si="98">VLOOKUP(A60,locations,3)</f>
-        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
+        <f t="shared" si="91"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="83"/>
-        <v>Australia/Melbourne</v>
+        <f t="shared" ref="D61:D62" si="97">VLOOKUP(A61,locations,4)</f>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E61" s="4">
-        <v>45220</v>
+        <v>45192</v>
       </c>
       <c r="F61" s="6">
-        <v>0.625</v>
+        <v>0.53472222222222221</v>
       </c>
       <c r="G61" s="4">
-        <f t="shared" si="96"/>
-        <v>45220</v>
+        <f t="shared" si="95"/>
+        <v>45192</v>
       </c>
       <c r="H61" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="97"/>
-        <v>Phillip Island</v>
+        <f t="shared" ref="I61:I62" si="98">VLOOKUP(A61,locations,2)</f>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" si="98"/>
-        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
+        <f t="shared" ref="J61:J62" si="99">VLOOKUP(A61,locations,3)</f>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="83"/>
-        <v>Australia/Melbourne</v>
+        <f t="shared" si="97"/>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E62" s="4">
-        <v>45221</v>
+        <v>45192</v>
       </c>
       <c r="F62" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="G62" s="4">
-        <f t="shared" si="96"/>
-        <v>45221</v>
+        <f t="shared" si="95"/>
+        <v>45192</v>
       </c>
       <c r="H62" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" ref="I62" si="99">VLOOKUP(A62,locations,2)</f>
-        <v>Phillip Island</v>
+        <f t="shared" si="98"/>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J62" t="str">
-        <f t="shared" ref="J62" si="100">VLOOKUP(A62,locations,3)</f>
-        <v>Animoca Brands Australian Motorcycle Grand Prix</v>
+        <f t="shared" si="99"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Bangkok</v>
+        <f t="shared" si="94"/>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E63" s="4">
-        <v>45227</v>
+        <v>45192</v>
       </c>
       <c r="F63" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.625</v>
       </c>
       <c r="G63" s="4">
-        <f t="shared" ref="G63:G65" si="101">E63</f>
-        <v>45227</v>
+        <f t="shared" si="95"/>
+        <v>45192</v>
       </c>
       <c r="H63" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" ref="I63:I64" si="102">VLOOKUP(A63,locations,2)</f>
-        <v>Chang International Circuit</v>
+        <f t="shared" si="96"/>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" ref="J63:J64" si="103">VLOOKUP(A63,locations,3)</f>
-        <v>OR Thailand Grand Prix</v>
+        <f t="shared" si="91"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Bangkok</v>
+        <f t="shared" ref="D64:D65" si="100">VLOOKUP(A64,locations,4)</f>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E64" s="4">
-        <v>45227</v>
+        <v>45193</v>
       </c>
       <c r="F64" s="6">
-        <v>0.625</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="G64" s="4">
-        <f t="shared" si="101"/>
-        <v>45227</v>
+        <f t="shared" si="95"/>
+        <v>45193</v>
       </c>
       <c r="H64" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.54861111111111105</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="102"/>
-        <v>Chang International Circuit</v>
+        <f t="shared" ref="I64:I65" si="101">VLOOKUP(A64,locations,2)</f>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" si="103"/>
-        <v>OR Thailand Grand Prix</v>
+        <f t="shared" ref="J64:J65" si="102">VLOOKUP(A64,locations,3)</f>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Bangkok</v>
+        <f t="shared" si="100"/>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E65" s="4">
-        <v>45228</v>
+        <v>45193</v>
       </c>
       <c r="F65" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="G65" s="4">
+        <f t="shared" si="95"/>
+        <v>45193</v>
+      </c>
+      <c r="H65" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I65" t="str">
         <f t="shared" si="101"/>
-        <v>45228</v>
-      </c>
-      <c r="H65" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I65" t="str">
-        <f t="shared" ref="I65" si="104">VLOOKUP(A65,locations,2)</f>
-        <v>Chang International Circuit</v>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" ref="J65" si="105">VLOOKUP(A65,locations,3)</f>
-        <v>OR Thailand Grand Prix</v>
+        <f t="shared" si="102"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Kuala_Lumpur</v>
+        <f t="shared" si="94"/>
+        <v>Asia/Kolkata</v>
       </c>
       <c r="E66" s="4">
-        <v>45241</v>
+        <v>45193</v>
       </c>
       <c r="F66" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="G66" s="4">
-        <f t="shared" ref="G66:G68" si="106">E66</f>
-        <v>45241</v>
+        <f t="shared" si="95"/>
+        <v>45193</v>
       </c>
       <c r="H66" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.68055555555555547</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" ref="I66:I67" si="107">VLOOKUP(A66,locations,2)</f>
-        <v>Sepang International Circuit</v>
+        <f t="shared" si="96"/>
+        <v>Buddh International Circuit</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" ref="J66:J67" si="108">VLOOKUP(A66,locations,3)</f>
-        <v>PETRONAS Grand Prix of Malaysia</v>
+        <f t="shared" si="91"/>
+        <v>Grand Prix of India</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Kuala_Lumpur</v>
+        <f t="shared" si="94"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E67" s="4">
-        <v>45241</v>
+        <v>45199</v>
       </c>
       <c r="F67" s="6">
-        <v>0.625</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G67" s="4">
-        <f t="shared" si="106"/>
-        <v>45241</v>
+        <f t="shared" ref="G67:G73" si="103">E67</f>
+        <v>45199</v>
       </c>
       <c r="H67" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="107"/>
-        <v>Sepang International Circuit</v>
+        <f t="shared" ref="I67:I70" si="104">VLOOKUP(A67,locations,2)</f>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" si="108"/>
-        <v>PETRONAS Grand Prix of Malaysia</v>
+        <f t="shared" ref="J67:J70" si="105">VLOOKUP(A67,locations,3)</f>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Kuala_Lumpur</v>
+        <f t="shared" si="94"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E68" s="4">
-        <v>45242</v>
+        <v>45199</v>
       </c>
       <c r="F68" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.53472222222222221</v>
       </c>
       <c r="G68" s="4">
-        <f t="shared" si="106"/>
-        <v>45242</v>
+        <f t="shared" si="103"/>
+        <v>45199</v>
       </c>
       <c r="H68" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.5625</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" ref="I68" si="109">VLOOKUP(A68,locations,2)</f>
-        <v>Sepang International Circuit</v>
+        <f t="shared" ref="I68:I69" si="106">VLOOKUP(A68,locations,2)</f>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J68" t="str">
-        <f t="shared" ref="J68" si="110">VLOOKUP(A68,locations,3)</f>
-        <v>PETRONAS Grand Prix of Malaysia</v>
+        <f t="shared" ref="J68:J69" si="107">VLOOKUP(A68,locations,3)</f>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Qatar</v>
+        <f t="shared" si="94"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E69" s="4">
-        <v>45248</v>
+        <v>45199</v>
       </c>
       <c r="F69" s="6">
-        <v>0.65972222222222221</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="G69" s="4">
-        <f>E69</f>
-        <v>45248</v>
+        <f t="shared" si="103"/>
+        <v>45199</v>
       </c>
       <c r="H69" s="6">
-        <v>0.6875</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" ref="I69:I70" si="111">VLOOKUP(A69,locations,2)</f>
-        <v>Losail International Circuit</v>
+        <f t="shared" si="106"/>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" ref="J69:J70" si="112">VLOOKUP(A69,locations,3)</f>
-        <v>Grand Prix of Qatar</v>
+        <f t="shared" si="107"/>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Qatar</v>
+        <f t="shared" si="94"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E70" s="4">
-        <v>45248</v>
+        <v>45199</v>
       </c>
       <c r="F70" s="6">
-        <v>0.83333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="G70" s="4">
-        <f>E70</f>
-        <v>45248</v>
+        <f t="shared" si="103"/>
+        <v>45199</v>
       </c>
       <c r="H70" s="6">
-        <v>0.85416666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="111"/>
-        <v>Losail International Circuit</v>
+        <f t="shared" si="104"/>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" si="112"/>
-        <v>Grand Prix of Qatar</v>
+        <f t="shared" si="105"/>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="83"/>
-        <v>Asia/Qatar</v>
+        <f t="shared" ref="D71:D72" si="108">VLOOKUP(A71,locations,4)</f>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E71" s="4">
-        <v>45249</v>
+        <v>45200</v>
       </c>
       <c r="F71" s="6">
-        <v>0.83333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="G71" s="4">
-        <f>E71</f>
-        <v>45249</v>
+        <f t="shared" si="103"/>
+        <v>45200</v>
       </c>
       <c r="H71" s="6">
-        <v>0.86805555555555547</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" ref="I71" si="113">VLOOKUP(A71,locations,2)</f>
-        <v>Losail International Circuit</v>
+        <f t="shared" ref="I71:I72" si="109">VLOOKUP(A71,locations,2)</f>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" ref="J71" si="114">VLOOKUP(A71,locations,3)</f>
-        <v>Grand Prix of Qatar</v>
+        <f t="shared" ref="J71:J72" si="110">VLOOKUP(A71,locations,3)</f>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="83"/>
-        <v>Europe/Madrid</v>
+        <f t="shared" si="108"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E72" s="4">
-        <v>45255</v>
+        <v>45200</v>
       </c>
       <c r="F72" s="6">
-        <v>0.4513888888888889</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="G72" s="4">
-        <f t="shared" ref="G72:G74" si="115">E72</f>
-        <v>45255</v>
+        <f t="shared" si="103"/>
+        <v>45200</v>
       </c>
       <c r="H72" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.60069444444444442</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" ref="I72:I73" si="116">VLOOKUP(A72,locations,2)</f>
-        <v>Circuit Ricardo Tormo</v>
+        <f t="shared" si="109"/>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J72" t="str">
-        <f t="shared" ref="J72:J73" si="117">VLOOKUP(A72,locations,3)</f>
-        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+        <f t="shared" si="110"/>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" ref="D73" si="118">VLOOKUP(A73,locations,4)</f>
-        <v>Europe/Madrid</v>
+        <f t="shared" si="94"/>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="E73" s="4">
-        <v>45255</v>
+        <v>45200</v>
       </c>
       <c r="F73" s="6">
         <v>0.625</v>
       </c>
       <c r="G73" s="4">
-        <f t="shared" si="115"/>
-        <v>45255</v>
+        <f t="shared" si="103"/>
+        <v>45200</v>
       </c>
       <c r="H73" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="116"/>
-        <v>Circuit Ricardo Tormo</v>
+        <f t="shared" ref="I73" si="111">VLOOKUP(A73,locations,2)</f>
+        <v>Mobility Resort Motegi</v>
       </c>
       <c r="J73" t="str">
-        <f t="shared" si="117"/>
-        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+        <f t="shared" ref="J73" si="112">VLOOKUP(A73,locations,3)</f>
+        <v>Motul Grand Prix of Japan</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Jakarta</v>
+      </c>
+      <c r="E74" s="4">
+        <v>45213</v>
+      </c>
+      <c r="F74" s="6">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G74" s="4">
+        <f t="shared" ref="G74:G80" si="113">E74</f>
+        <v>45213</v>
+      </c>
+      <c r="H74" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I74" t="str">
+        <f t="shared" ref="I74:I77" si="114">VLOOKUP(A74,locations,2)</f>
+        <v>Mandalika International Street Circuit</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" ref="J74:J77" si="115">VLOOKUP(A74,locations,3)</f>
+        <v>Pertamina Grand Prix of Indonesia</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" ref="D75:D76" si="116">VLOOKUP(A75,locations,4)</f>
+        <v>Asia/Jakarta</v>
+      </c>
+      <c r="E75" s="4">
+        <v>45213</v>
+      </c>
+      <c r="F75" s="6">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="G75" s="4">
+        <f t="shared" si="113"/>
+        <v>45213</v>
+      </c>
+      <c r="H75" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" ref="I75:I76" si="117">VLOOKUP(A75,locations,2)</f>
+        <v>Mandalika International Street Circuit</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" ref="J75:J76" si="118">VLOOKUP(A75,locations,3)</f>
+        <v>Pertamina Grand Prix of Indonesia</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="116"/>
+        <v>Asia/Jakarta</v>
+      </c>
+      <c r="E76" s="4">
+        <v>45213</v>
+      </c>
+      <c r="F76" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G76" s="4">
+        <f t="shared" si="113"/>
+        <v>45213</v>
+      </c>
+      <c r="H76" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="117"/>
+        <v>Mandalika International Street Circuit</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="118"/>
+        <v>Pertamina Grand Prix of Indonesia</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Jakarta</v>
+      </c>
+      <c r="E77" s="4">
+        <v>45213</v>
+      </c>
+      <c r="F77" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G77" s="4">
+        <f t="shared" si="113"/>
+        <v>45213</v>
+      </c>
+      <c r="H77" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="114"/>
+        <v>Mandalika International Street Circuit</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="115"/>
+        <v>Pertamina Grand Prix of Indonesia</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" ref="D78:D79" si="119">VLOOKUP(A78,locations,4)</f>
+        <v>Asia/Jakarta</v>
+      </c>
+      <c r="E78" s="4">
+        <v>45214</v>
+      </c>
+      <c r="F78" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G78" s="4">
+        <f t="shared" si="113"/>
+        <v>45214</v>
+      </c>
+      <c r="H78" s="6">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="I78" t="str">
+        <f t="shared" ref="I78:I79" si="120">VLOOKUP(A78,locations,2)</f>
+        <v>Mandalika International Street Circuit</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" ref="J78:J79" si="121">VLOOKUP(A78,locations,3)</f>
+        <v>Pertamina Grand Prix of Indonesia</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="119"/>
+        <v>Asia/Jakarta</v>
+      </c>
+      <c r="E79" s="4">
+        <v>45214</v>
+      </c>
+      <c r="F79" s="6">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G79" s="4">
+        <f t="shared" si="113"/>
+        <v>45214</v>
+      </c>
+      <c r="H79" s="6">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="I79" t="str">
+        <f t="shared" si="120"/>
+        <v>Mandalika International Street Circuit</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="121"/>
+        <v>Pertamina Grand Prix of Indonesia</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Jakarta</v>
+      </c>
+      <c r="E80" s="4">
+        <v>45214</v>
+      </c>
+      <c r="F80" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G80" s="4">
+        <f t="shared" si="113"/>
+        <v>45214</v>
+      </c>
+      <c r="H80" s="6">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="I80" t="str">
+        <f t="shared" ref="I80" si="122">VLOOKUP(A80,locations,2)</f>
+        <v>Mandalika International Street Circuit</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" ref="J80" si="123">VLOOKUP(A80,locations,3)</f>
+        <v>Pertamina Grand Prix of Indonesia</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="94"/>
+        <v>Australia/Melbourne</v>
+      </c>
+      <c r="E81" s="4">
+        <v>45220</v>
+      </c>
+      <c r="F81" s="6">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G81" s="4">
+        <f t="shared" ref="G81:G87" si="124">E81</f>
+        <v>45220</v>
+      </c>
+      <c r="H81" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I81" t="str">
+        <f t="shared" ref="I81:I84" si="125">VLOOKUP(A81,locations,2)</f>
+        <v>Phillip Island</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" ref="J81:J84" si="126">VLOOKUP(A81,locations,3)</f>
+        <v>MotoGP Guru by Gryfyn Australian Motorcycle Grand Prix</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" ref="D82:D83" si="127">VLOOKUP(A82,locations,4)</f>
+        <v>Australia/Melbourne</v>
+      </c>
+      <c r="E82" s="4">
+        <v>45220</v>
+      </c>
+      <c r="F82" s="6">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="G82" s="4">
+        <f t="shared" si="124"/>
+        <v>45220</v>
+      </c>
+      <c r="H82" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="I82" t="str">
+        <f t="shared" ref="I82:I83" si="128">VLOOKUP(A82,locations,2)</f>
+        <v>Phillip Island</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" ref="J82:J83" si="129">VLOOKUP(A82,locations,3)</f>
+        <v>MotoGP Guru by Gryfyn Australian Motorcycle Grand Prix</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>35</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="127"/>
+        <v>Australia/Melbourne</v>
+      </c>
+      <c r="E83" s="4">
+        <v>45220</v>
+      </c>
+      <c r="F83" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G83" s="4">
+        <f t="shared" si="124"/>
+        <v>45220</v>
+      </c>
+      <c r="H83" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="128"/>
+        <v>Phillip Island</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="129"/>
+        <v>MotoGP Guru by Gryfyn Australian Motorcycle Grand Prix</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>35</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="94"/>
+        <v>Australia/Melbourne</v>
+      </c>
+      <c r="E84" s="4">
+        <v>45220</v>
+      </c>
+      <c r="F84" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G84" s="4">
+        <f t="shared" si="124"/>
+        <v>45220</v>
+      </c>
+      <c r="H84" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="125"/>
+        <v>Phillip Island</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="126"/>
+        <v>MotoGP Guru by Gryfyn Australian Motorcycle Grand Prix</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>35</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" ref="D85:D86" si="130">VLOOKUP(A85,locations,4)</f>
+        <v>Australia/Melbourne</v>
+      </c>
+      <c r="E85" s="4">
+        <v>45221</v>
+      </c>
+      <c r="F85" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G85" s="4">
+        <f t="shared" si="124"/>
+        <v>45221</v>
+      </c>
+      <c r="H85" s="6">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" ref="I85:I87" si="131">VLOOKUP(A85,locations,2)</f>
+        <v>Phillip Island</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" ref="J85:J87" si="132">VLOOKUP(A85,locations,3)</f>
+        <v>MotoGP Guru by Gryfyn Australian Motorcycle Grand Prix</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>35</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="130"/>
+        <v>Australia/Melbourne</v>
+      </c>
+      <c r="E86" s="4">
+        <v>45221</v>
+      </c>
+      <c r="F86" s="6">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G86" s="4">
+        <f t="shared" si="124"/>
+        <v>45221</v>
+      </c>
+      <c r="H86" s="6">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" si="131"/>
+        <v>Phillip Island</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="132"/>
+        <v>MotoGP Guru by Gryfyn Australian Motorcycle Grand Prix</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>35</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="94"/>
+        <v>Australia/Melbourne</v>
+      </c>
+      <c r="E87" s="4">
+        <v>45221</v>
+      </c>
+      <c r="F87" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G87" s="4">
+        <f t="shared" si="124"/>
+        <v>45221</v>
+      </c>
+      <c r="H87" s="6">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="131"/>
+        <v>Phillip Island</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="132"/>
+        <v>MotoGP Guru by Gryfyn Australian Motorcycle Grand Prix</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>34</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Bangkok</v>
+      </c>
+      <c r="E88" s="4">
+        <v>45227</v>
+      </c>
+      <c r="F88" s="6">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G88" s="4">
+        <f t="shared" ref="G88:G94" si="133">E88</f>
+        <v>45227</v>
+      </c>
+      <c r="H88" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I88" t="str">
+        <f t="shared" ref="I88:I91" si="134">VLOOKUP(A88,locations,2)</f>
+        <v>Chang International Circuit</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" ref="J88:J91" si="135">VLOOKUP(A88,locations,3)</f>
+        <v>OR Thailand Grand Prix</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>34</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" ref="D89:D90" si="136">VLOOKUP(A89,locations,4)</f>
+        <v>Asia/Bangkok</v>
+      </c>
+      <c r="E89" s="4">
+        <v>45227</v>
+      </c>
+      <c r="F89" s="6">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="G89" s="4">
+        <f t="shared" si="133"/>
+        <v>45227</v>
+      </c>
+      <c r="H89" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="I89" t="str">
+        <f t="shared" ref="I89:I90" si="137">VLOOKUP(A89,locations,2)</f>
+        <v>Chang International Circuit</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" ref="J89:J90" si="138">VLOOKUP(A89,locations,3)</f>
+        <v>OR Thailand Grand Prix</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>34</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="136"/>
+        <v>Asia/Bangkok</v>
+      </c>
+      <c r="E90" s="4">
+        <v>45227</v>
+      </c>
+      <c r="F90" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G90" s="4">
+        <f t="shared" si="133"/>
+        <v>45227</v>
+      </c>
+      <c r="H90" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="137"/>
+        <v>Chang International Circuit</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="138"/>
+        <v>OR Thailand Grand Prix</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>34</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Bangkok</v>
+      </c>
+      <c r="E91" s="4">
+        <v>45227</v>
+      </c>
+      <c r="F91" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G91" s="4">
+        <f t="shared" si="133"/>
+        <v>45227</v>
+      </c>
+      <c r="H91" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I91" t="str">
+        <f t="shared" si="134"/>
+        <v>Chang International Circuit</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" si="135"/>
+        <v>OR Thailand Grand Prix</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>34</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" ref="D92:D93" si="139">VLOOKUP(A92,locations,4)</f>
+        <v>Asia/Bangkok</v>
+      </c>
+      <c r="E92" s="4">
+        <v>45228</v>
+      </c>
+      <c r="F92" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G92" s="4">
+        <f t="shared" si="133"/>
+        <v>45228</v>
+      </c>
+      <c r="H92" s="6">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" ref="I92:I93" si="140">VLOOKUP(A92,locations,2)</f>
+        <v>Chang International Circuit</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" ref="J92:J93" si="141">VLOOKUP(A92,locations,3)</f>
+        <v>OR Thailand Grand Prix</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>34</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="139"/>
+        <v>Asia/Bangkok</v>
+      </c>
+      <c r="E93" s="4">
+        <v>45228</v>
+      </c>
+      <c r="F93" s="6">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G93" s="4">
+        <f t="shared" si="133"/>
+        <v>45228</v>
+      </c>
+      <c r="H93" s="6">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" si="140"/>
+        <v>Chang International Circuit</v>
+      </c>
+      <c r="J93" t="str">
+        <f t="shared" si="141"/>
+        <v>OR Thailand Grand Prix</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>34</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Bangkok</v>
+      </c>
+      <c r="E94" s="4">
+        <v>45228</v>
+      </c>
+      <c r="F94" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G94" s="4">
+        <f t="shared" si="133"/>
+        <v>45228</v>
+      </c>
+      <c r="H94" s="6">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="I94" t="str">
+        <f t="shared" ref="I94" si="142">VLOOKUP(A94,locations,2)</f>
+        <v>Chang International Circuit</v>
+      </c>
+      <c r="J94" t="str">
+        <f t="shared" ref="J94" si="143">VLOOKUP(A94,locations,3)</f>
+        <v>OR Thailand Grand Prix</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>36</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Kuala_Lumpur</v>
+      </c>
+      <c r="E95" s="4">
+        <v>45241</v>
+      </c>
+      <c r="F95" s="6">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G95" s="4">
+        <f t="shared" ref="G95:G101" si="144">E95</f>
+        <v>45241</v>
+      </c>
+      <c r="H95" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" ref="I95:I98" si="145">VLOOKUP(A95,locations,2)</f>
+        <v>Sepang International Circuit</v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" ref="J95:J98" si="146">VLOOKUP(A95,locations,3)</f>
+        <v>PETRONAS Grand Prix of Malaysia</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>36</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" ref="D96:D97" si="147">VLOOKUP(A96,locations,4)</f>
+        <v>Asia/Kuala_Lumpur</v>
+      </c>
+      <c r="E96" s="4">
+        <v>45241</v>
+      </c>
+      <c r="F96" s="6">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="G96" s="4">
+        <f t="shared" si="144"/>
+        <v>45241</v>
+      </c>
+      <c r="H96" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" ref="I96:I97" si="148">VLOOKUP(A96,locations,2)</f>
+        <v>Sepang International Circuit</v>
+      </c>
+      <c r="J96" t="str">
+        <f t="shared" ref="J96:J97" si="149">VLOOKUP(A96,locations,3)</f>
+        <v>PETRONAS Grand Prix of Malaysia</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>36</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="147"/>
+        <v>Asia/Kuala_Lumpur</v>
+      </c>
+      <c r="E97" s="4">
+        <v>45241</v>
+      </c>
+      <c r="F97" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G97" s="4">
+        <f t="shared" si="144"/>
+        <v>45241</v>
+      </c>
+      <c r="H97" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="148"/>
+        <v>Sepang International Circuit</v>
+      </c>
+      <c r="J97" t="str">
+        <f t="shared" si="149"/>
+        <v>PETRONAS Grand Prix of Malaysia</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>36</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Kuala_Lumpur</v>
+      </c>
+      <c r="E98" s="4">
+        <v>45241</v>
+      </c>
+      <c r="F98" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G98" s="4">
+        <f t="shared" si="144"/>
+        <v>45241</v>
+      </c>
+      <c r="H98" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="145"/>
+        <v>Sepang International Circuit</v>
+      </c>
+      <c r="J98" t="str">
+        <f t="shared" si="146"/>
+        <v>PETRONAS Grand Prix of Malaysia</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>36</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" ref="D99:D100" si="150">VLOOKUP(A99,locations,4)</f>
+        <v>Asia/Kuala_Lumpur</v>
+      </c>
+      <c r="E99" s="4">
+        <v>45242</v>
+      </c>
+      <c r="F99" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G99" s="4">
+        <f t="shared" si="144"/>
+        <v>45242</v>
+      </c>
+      <c r="H99" s="6">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="I99" t="str">
+        <f t="shared" ref="I99:I100" si="151">VLOOKUP(A99,locations,2)</f>
+        <v>Sepang International Circuit</v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" ref="J99:J100" si="152">VLOOKUP(A99,locations,3)</f>
+        <v>PETRONAS Grand Prix of Malaysia</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>36</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="150"/>
+        <v>Asia/Kuala_Lumpur</v>
+      </c>
+      <c r="E100" s="4">
+        <v>45242</v>
+      </c>
+      <c r="F100" s="6">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G100" s="4">
+        <f t="shared" si="144"/>
+        <v>45242</v>
+      </c>
+      <c r="H100" s="6">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="I100" t="str">
+        <f t="shared" si="151"/>
+        <v>Sepang International Circuit</v>
+      </c>
+      <c r="J100" t="str">
+        <f t="shared" si="152"/>
+        <v>PETRONAS Grand Prix of Malaysia</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>36</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Kuala_Lumpur</v>
+      </c>
+      <c r="E101" s="4">
+        <v>45242</v>
+      </c>
+      <c r="F101" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G101" s="4">
+        <f t="shared" si="144"/>
+        <v>45242</v>
+      </c>
+      <c r="H101" s="6">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="I101" t="str">
+        <f t="shared" ref="I101" si="153">VLOOKUP(A101,locations,2)</f>
+        <v>Sepang International Circuit</v>
+      </c>
+      <c r="J101" t="str">
+        <f t="shared" ref="J101" si="154">VLOOKUP(A101,locations,3)</f>
+        <v>PETRONAS Grand Prix of Malaysia</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>17</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E102" s="4">
+        <v>45248</v>
+      </c>
+      <c r="F102" s="6">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="G102" s="4">
+        <f>E102</f>
+        <v>45248</v>
+      </c>
+      <c r="H102" s="6">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="I102" t="str">
+        <f t="shared" ref="I102:I105" si="155">VLOOKUP(A102,locations,2)</f>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J102" t="str">
+        <f t="shared" ref="J102:J105" si="156">VLOOKUP(A102,locations,3)</f>
+        <v>Qatar Airways Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" ref="D103:D104" si="157">VLOOKUP(A103,locations,4)</f>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E103" s="4">
+        <v>45248</v>
+      </c>
+      <c r="F103" s="6">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="G103" s="4">
+        <f t="shared" ref="G103:G104" si="158">E103</f>
+        <v>45248</v>
+      </c>
+      <c r="H103" s="6">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="I103" t="str">
+        <f t="shared" ref="I103:I104" si="159">VLOOKUP(A103,locations,2)</f>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J103" t="str">
+        <f t="shared" ref="J103:J104" si="160">VLOOKUP(A103,locations,3)</f>
+        <v>Qatar Airways Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="157"/>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E104" s="4">
+        <v>45248</v>
+      </c>
+      <c r="F104" s="6">
+        <v>0.78125</v>
+      </c>
+      <c r="G104" s="4">
+        <f t="shared" si="158"/>
+        <v>45248</v>
+      </c>
+      <c r="H104" s="6">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="I104" t="str">
+        <f t="shared" si="159"/>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J104" t="str">
+        <f t="shared" si="160"/>
+        <v>Qatar Airways Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>17</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E105" s="4">
+        <v>45248</v>
+      </c>
+      <c r="F105" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G105" s="4">
+        <f>E105</f>
+        <v>45248</v>
+      </c>
+      <c r="H105" s="6">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="I105" t="str">
+        <f t="shared" si="155"/>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J105" t="str">
+        <f t="shared" si="156"/>
+        <v>Qatar Airways Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>17</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" ref="D106:D107" si="161">VLOOKUP(A106,locations,4)</f>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E106" s="4">
+        <v>45249</v>
+      </c>
+      <c r="F106" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G106" s="4">
+        <f>E106</f>
+        <v>45249</v>
+      </c>
+      <c r="H106" s="6">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="I106" t="str">
+        <f t="shared" ref="I106:I107" si="162">VLOOKUP(A106,locations,2)</f>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J106" t="str">
+        <f t="shared" ref="J106:J107" si="163">VLOOKUP(A106,locations,3)</f>
+        <v>Qatar Airways Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>17</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="161"/>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E107" s="4">
+        <v>45249</v>
+      </c>
+      <c r="F107" s="6">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="G107" s="4">
+        <f>E107</f>
+        <v>45249</v>
+      </c>
+      <c r="H107" s="6">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="I107" t="str">
+        <f t="shared" si="162"/>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J107" t="str">
+        <f t="shared" si="163"/>
+        <v>Qatar Airways Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>17</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="94"/>
+        <v>Asia/Qatar</v>
+      </c>
+      <c r="E108" s="4">
+        <v>45249</v>
+      </c>
+      <c r="F108" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G108" s="4">
+        <f>E108</f>
+        <v>45249</v>
+      </c>
+      <c r="H108" s="6">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="I108" t="str">
+        <f t="shared" ref="I108" si="164">VLOOKUP(A108,locations,2)</f>
+        <v>Losail International Circuit</v>
+      </c>
+      <c r="J108" t="str">
+        <f t="shared" ref="J108" si="165">VLOOKUP(A108,locations,3)</f>
+        <v>Qatar Airways Grand Prix of Qatar</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>37</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C74" s="3" t="s">
+      <c r="B109" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="94"/>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E109" s="4">
+        <v>45255</v>
+      </c>
+      <c r="F109" s="6">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G109" s="4">
+        <f t="shared" ref="G109:G115" si="166">E109</f>
+        <v>45255</v>
+      </c>
+      <c r="H109" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I109" t="str">
+        <f t="shared" ref="I109:I112" si="167">VLOOKUP(A109,locations,2)</f>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J109" t="str">
+        <f t="shared" ref="J109:J112" si="168">VLOOKUP(A109,locations,3)</f>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>37</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="94"/>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E110" s="4">
+        <v>45255</v>
+      </c>
+      <c r="F110" s="6">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="G110" s="4">
+        <f t="shared" si="166"/>
+        <v>45255</v>
+      </c>
+      <c r="H110" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="I110" t="str">
+        <f t="shared" ref="I110:I111" si="169">VLOOKUP(A110,locations,2)</f>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J110" t="str">
+        <f t="shared" ref="J110:J111" si="170">VLOOKUP(A110,locations,3)</f>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>37</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="94"/>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E111" s="4">
+        <v>45255</v>
+      </c>
+      <c r="F111" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G111" s="4">
+        <f t="shared" si="166"/>
+        <v>45255</v>
+      </c>
+      <c r="H111" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I111" t="str">
+        <f t="shared" si="169"/>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J111" t="str">
+        <f t="shared" si="170"/>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>37</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" ref="D112:D114" si="171">VLOOKUP(A112,locations,4)</f>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E112" s="4">
+        <v>45255</v>
+      </c>
+      <c r="F112" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G112" s="4">
+        <f t="shared" si="166"/>
+        <v>45255</v>
+      </c>
+      <c r="H112" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I112" t="str">
+        <f t="shared" si="167"/>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J112" t="str">
+        <f t="shared" si="168"/>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>37</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D74" t="str">
-        <f t="shared" ref="D74" si="119">VLOOKUP(A74,locations,4)</f>
+      <c r="D113" t="str">
+        <f t="shared" si="171"/>
         <v>Europe/Madrid</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E113" s="4">
         <v>45256</v>
       </c>
-      <c r="F74" s="6">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G74" s="4">
-        <f t="shared" si="115"/>
+      <c r="F113" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G113" s="4">
+        <f t="shared" si="166"/>
         <v>45256</v>
       </c>
-      <c r="H74" s="6">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="I74" t="str">
-        <f t="shared" ref="I74" si="120">VLOOKUP(A74,locations,2)</f>
+      <c r="H113" s="6">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="I113" t="str">
+        <f t="shared" ref="I113:I114" si="172">VLOOKUP(A113,locations,2)</f>
         <v>Circuit Ricardo Tormo</v>
       </c>
-      <c r="J74" t="str">
-        <f t="shared" ref="J74" si="121">VLOOKUP(A74,locations,3)</f>
+      <c r="J113" t="str">
+        <f t="shared" ref="J113:J114" si="173">VLOOKUP(A113,locations,3)</f>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>37</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="171"/>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E114" s="4">
+        <v>45256</v>
+      </c>
+      <c r="F114" s="6">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="G114" s="4">
+        <f t="shared" si="166"/>
+        <v>45256</v>
+      </c>
+      <c r="H114" s="6">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I114" t="str">
+        <f t="shared" si="172"/>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J114" t="str">
+        <f t="shared" si="173"/>
+        <v>Gran Premio Motul de la Comunitat Valenciana</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>37</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" ref="D115" si="174">VLOOKUP(A115,locations,4)</f>
+        <v>Europe/Madrid</v>
+      </c>
+      <c r="E115" s="4">
+        <v>45256</v>
+      </c>
+      <c r="F115" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="G115" s="4">
+        <f t="shared" si="166"/>
+        <v>45256</v>
+      </c>
+      <c r="H115" s="6">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="I115" t="str">
+        <f t="shared" ref="I115" si="175">VLOOKUP(A115,locations,2)</f>
+        <v>Circuit Ricardo Tormo</v>
+      </c>
+      <c r="J115" t="str">
+        <f t="shared" ref="J115" si="176">VLOOKUP(A115,locations,3)</f>
         <v>Gran Premio Motul de la Comunitat Valenciana</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A79:A82 A2:A74" xr:uid="{F03BE25C-DA6F-6246-A9E5-DB905318EDFD}">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A120:A123 A2:A115" xr:uid="{F03BE25C-DA6F-6246-A9E5-DB905318EDFD}">
       <formula1>countries</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79:B82 B2:B74" xr:uid="{0EA54380-98F5-E141-93FA-55C8FE75E20E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B120:B123 B2:B115" xr:uid="{0EA54380-98F5-E141-93FA-55C8FE75E20E}">
       <formula1>categories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C79:C82 C2:C74" xr:uid="{8F2CDCBC-21D9-4843-9F7D-D70F3A2F785B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C120:C123 C2:C115" xr:uid="{8F2CDCBC-21D9-4843-9F7D-D70F3A2F785B}">
       <formula1>sessions</formula1>
     </dataValidation>
   </dataValidations>
@@ -3455,10 +4927,10 @@
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3486,13 +4958,13 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -3506,19 +4978,19 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3526,13 +4998,13 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -3546,19 +5018,19 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
         <v>71</v>
       </c>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3566,13 +5038,13 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3580,13 +5052,13 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3594,13 +5066,13 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
         <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3608,13 +5080,13 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" t="s">
         <v>62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3622,27 +5094,27 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" t="s">
         <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" t="s">
         <v>106</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -3650,13 +5122,13 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -3664,13 +5136,13 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" t="s">
         <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -3678,27 +5150,27 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" t="s">
         <v>98</v>
-      </c>
-      <c r="D15" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -3706,13 +5178,13 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3720,13 +5192,13 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3734,13 +5206,13 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3751,10 +5223,10 @@
         <v>40</v>
       </c>
       <c r="C19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" t="s">
         <v>43</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3762,13 +5234,13 @@
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3776,13 +5248,13 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
         <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3790,13 +5262,13 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3804,13 +5276,13 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
         <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -3818,13 +5290,13 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct Moto2 race times
</commit_message>
<xml_diff>
--- a/motogp/MotoGP.xlsx
+++ b/motogp/MotoGP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/motogp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0235E8C-7FC5-1F4F-9E3D-53D5C67D4411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F3BCA3B-8716-5840-BF36-D47F048F9870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="1900" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
+    <workbookView xWindow="3220" yWindow="1320" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
   <sheets>
     <sheet name="MotoGP" sheetId="1" r:id="rId1"/>
@@ -3341,7 +3341,7 @@
         <v>45200</v>
       </c>
       <c r="H72" s="6">
-        <v>0.60069444444444442</v>
+        <v>0.57986111111111105</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="109"/>

</xml_diff>

<commit_message>
Update times of Moto2 Race
</commit_message>
<xml_diff>
--- a/motogp/MotoGP.xlsx
+++ b/motogp/MotoGP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/motogp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F3BCA3B-8716-5840-BF36-D47F048F9870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D482F804-A95E-A04A-909C-D0561501EC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="1320" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -3593,7 +3593,7 @@
         <v>45214</v>
       </c>
       <c r="H79" s="6">
-        <v>0.55902777777777779</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" si="120"/>

</xml_diff>

<commit_message>
Change days for Australian Race and Sprint
</commit_message>
<xml_diff>
--- a/motogp/MotoGP.xlsx
+++ b/motogp/MotoGP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/motogp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D482F804-A95E-A04A-909C-D0561501EC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DA8B632-4DB8-0645-A162-88041A97BAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="1320" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -3756,7 +3756,7 @@
         <v>12</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="94"/>
@@ -3766,14 +3766,14 @@
         <v>45220</v>
       </c>
       <c r="F84" s="6">
-        <v>0.625</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="G84" s="4">
         <f t="shared" si="124"/>
         <v>45220</v>
       </c>
       <c r="H84" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I84" t="str">
         <f t="shared" si="125"/>
@@ -3802,14 +3802,14 @@
         <v>45221</v>
       </c>
       <c r="F85" s="6">
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="G85" s="4">
         <f t="shared" si="124"/>
         <v>45221</v>
       </c>
       <c r="H85" s="6">
-        <v>0.4861111111111111</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="I85" t="str">
         <f t="shared" ref="I85:I87" si="131">VLOOKUP(A85,locations,2)</f>
@@ -3838,14 +3838,14 @@
         <v>45221</v>
       </c>
       <c r="F86" s="6">
-        <v>0.51041666666666663</v>
+        <v>0.46875</v>
       </c>
       <c r="G86" s="4">
         <f t="shared" si="124"/>
         <v>45221</v>
       </c>
       <c r="H86" s="6">
-        <v>0.55902777777777779</v>
+        <v>0.5</v>
       </c>
       <c r="I86" t="str">
         <f t="shared" si="131"/>
@@ -3864,7 +3864,7 @@
         <v>12</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="94"/>
@@ -3874,14 +3874,14 @@
         <v>45221</v>
       </c>
       <c r="F87" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="G87" s="4">
         <f t="shared" si="124"/>
         <v>45221</v>
       </c>
       <c r="H87" s="6">
-        <v>0.61805555555555558</v>
+        <v>0.5625</v>
       </c>
       <c r="I87" t="str">
         <f t="shared" si="131"/>
@@ -4902,7 +4902,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A120:A123 A2:A115" xr:uid="{F03BE25C-DA6F-6246-A9E5-DB905318EDFD}">
       <formula1>countries</formula1>
     </dataValidation>

</xml_diff>